<commit_message>
changed from numpy to f strings in assignment 11
</commit_message>
<xml_diff>
--- a/01_studieplan_och_schema.xlsx
+++ b/01_studieplan_och_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsabellaGagner\Documents\Programming-projects\EC\ec-python-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02505D8-4229-4B19-AF26-D5485F03B379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5B7D25-B9D4-4D8F-82E9-D0A59314D2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="4320" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="180">
   <si>
     <t>Utbildning: Data Scientist</t>
   </si>
@@ -528,9 +528,6 @@
     <t>Main-metod, skripting, funktion, typing, konventioner, docstrings</t>
   </si>
   <si>
-    <t>Repetition vecka 1, skripting, terminalkommandon, argparse</t>
-  </si>
-  <si>
     <t>PP 8-10</t>
   </si>
   <si>
@@ -582,7 +579,7 @@
     <t>https://realpython.com/python-f-strings/#f-strings-a-new-and-improved-way-to-format-strings-in-python</t>
   </si>
   <si>
-    <t>Att skapa ett git-repo</t>
+    <t>Repetition vecka 1, terminalkommandon, argparse, att skapa ett git-repo</t>
   </si>
 </sst>
 </file>
@@ -1353,6 +1350,201 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1383,211 +1575,55 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1598,52 +1634,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2018,9 +2015,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3:I5"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -2085,7 +2082,7 @@
       <c r="N1" s="74"/>
     </row>
     <row r="2" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="144" t="s">
+      <c r="A2" s="156" t="s">
         <v>70</v>
       </c>
       <c r="B2" s="75">
@@ -2107,11 +2104,11 @@
       <c r="N2" s="77"/>
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="144"/>
-      <c r="B3" s="164">
+      <c r="A3" s="156"/>
+      <c r="B3" s="185">
         <v>44432</v>
       </c>
-      <c r="C3" s="163" t="s">
+      <c r="C3" s="184" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="51" t="s">
@@ -2129,10 +2126,10 @@
       <c r="H3" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="163" t="s">
+      <c r="I3" s="184" t="s">
         <v>160</v>
       </c>
-      <c r="J3" s="163" t="s">
+      <c r="J3" s="184" t="s">
         <v>46</v>
       </c>
       <c r="K3" s="79"/>
@@ -2145,9 +2142,9 @@
       <c r="N3" s="77"/>
     </row>
     <row r="4" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="144"/>
-      <c r="B4" s="164"/>
-      <c r="C4" s="163"/>
+      <c r="A4" s="156"/>
+      <c r="B4" s="185"/>
+      <c r="C4" s="184"/>
       <c r="D4" s="51" t="s">
         <v>22</v>
       </c>
@@ -2163,8 +2160,8 @@
       <c r="H4" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="163"/>
-      <c r="J4" s="163"/>
+      <c r="I4" s="184"/>
+      <c r="J4" s="184"/>
       <c r="K4" s="79"/>
       <c r="L4" s="51"/>
       <c r="M4" s="51" t="s">
@@ -2173,9 +2170,9 @@
       <c r="N4" s="77"/>
     </row>
     <row r="5" spans="1:14" ht="27.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="144"/>
-      <c r="B5" s="164"/>
-      <c r="C5" s="163"/>
+      <c r="A5" s="156"/>
+      <c r="B5" s="185"/>
+      <c r="C5" s="184"/>
       <c r="D5" s="51" t="s">
         <v>58</v>
       </c>
@@ -2191,8 +2188,8 @@
       <c r="H5" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="163"/>
-      <c r="J5" s="163"/>
+      <c r="I5" s="184"/>
+      <c r="J5" s="184"/>
       <c r="K5" s="79"/>
       <c r="L5" s="51" t="s">
         <v>38</v>
@@ -2203,11 +2200,11 @@
       <c r="N5" s="77"/>
     </row>
     <row r="6" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="144"/>
-      <c r="B6" s="166">
+      <c r="A6" s="156"/>
+      <c r="B6" s="187">
         <v>44433</v>
       </c>
-      <c r="C6" s="150" t="s">
+      <c r="C6" s="191" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="55" t="s">
@@ -2225,10 +2222,10 @@
       <c r="H6" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="159" t="s">
+      <c r="I6" s="180" t="s">
         <v>148</v>
       </c>
-      <c r="J6" s="159" t="s">
+      <c r="J6" s="180" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="56"/>
@@ -2239,9 +2236,9 @@
       <c r="N6" s="77"/>
     </row>
     <row r="7" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="144"/>
-      <c r="B7" s="166"/>
-      <c r="C7" s="150"/>
+      <c r="A7" s="156"/>
+      <c r="B7" s="187"/>
+      <c r="C7" s="191"/>
       <c r="D7" s="55" t="s">
         <v>59</v>
       </c>
@@ -2253,8 +2250,8 @@
       <c r="H7" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="159"/>
-      <c r="J7" s="159"/>
+      <c r="I7" s="180"/>
+      <c r="J7" s="180"/>
       <c r="K7" s="56"/>
       <c r="L7" s="55"/>
       <c r="M7" s="55" t="s">
@@ -2263,7 +2260,7 @@
       <c r="N7" s="77"/>
     </row>
     <row r="8" spans="1:14" ht="25.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="144"/>
+      <c r="A8" s="156"/>
       <c r="B8" s="78">
         <v>44434</v>
       </c>
@@ -2295,11 +2292,11 @@
       <c r="N8" s="77"/>
     </row>
     <row r="9" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="144"/>
-      <c r="B9" s="166">
+      <c r="A9" s="156"/>
+      <c r="B9" s="187">
         <v>44435</v>
       </c>
-      <c r="C9" s="150" t="s">
+      <c r="C9" s="191" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="55" t="s">
@@ -2317,14 +2314,14 @@
       <c r="H9" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="159" t="s">
+      <c r="I9" s="180" t="s">
         <v>151</v>
       </c>
-      <c r="J9" s="159" t="s">
+      <c r="J9" s="180" t="s">
         <v>146</v>
       </c>
       <c r="K9" s="56"/>
-      <c r="L9" s="191" t="s">
+      <c r="L9" s="131" t="s">
         <v>152</v>
       </c>
       <c r="M9" s="55" t="s">
@@ -2333,9 +2330,9 @@
       <c r="N9" s="77"/>
     </row>
     <row r="10" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="144"/>
-      <c r="B10" s="166"/>
-      <c r="C10" s="150"/>
+      <c r="A10" s="156"/>
+      <c r="B10" s="187"/>
+      <c r="C10" s="191"/>
       <c r="D10" s="55" t="s">
         <v>63</v>
       </c>
@@ -2347,10 +2344,10 @@
       <c r="H10" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="159"/>
-      <c r="J10" s="159"/>
+      <c r="I10" s="180"/>
+      <c r="J10" s="180"/>
       <c r="K10" s="56"/>
-      <c r="L10" s="192"/>
+      <c r="L10" s="132"/>
       <c r="M10" s="55" t="s">
         <v>143</v>
       </c>
@@ -2376,13 +2373,13 @@
       <c r="N11" s="77"/>
     </row>
     <row r="12" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="144" t="s">
+      <c r="A12" s="156" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="142">
+      <c r="B12" s="160">
         <v>44438</v>
       </c>
-      <c r="C12" s="153" t="s">
+      <c r="C12" s="174" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="52" t="s">
@@ -2395,18 +2392,18 @@
         <v>28</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="H12" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="I12" s="139" t="s">
+      <c r="I12" s="137" t="s">
+        <v>162</v>
+      </c>
+      <c r="J12" s="137" t="s">
         <v>163</v>
       </c>
-      <c r="J12" s="139" t="s">
-        <v>164</v>
-      </c>
-      <c r="K12" s="134" t="s">
+      <c r="K12" s="199" t="s">
         <v>124</v>
       </c>
       <c r="L12" s="53"/>
@@ -2416,9 +2413,9 @@
       <c r="N12" s="77"/>
     </row>
     <row r="13" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="145"/>
-      <c r="B13" s="143"/>
-      <c r="C13" s="156"/>
+      <c r="A13" s="157"/>
+      <c r="B13" s="161"/>
+      <c r="C13" s="175"/>
       <c r="D13" s="50" t="s">
         <v>63</v>
       </c>
@@ -2426,15 +2423,13 @@
         <v>1</v>
       </c>
       <c r="F13" s="50"/>
-      <c r="G13" s="50" t="s">
-        <v>180</v>
-      </c>
+      <c r="G13" s="50"/>
       <c r="H13" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="140"/>
-      <c r="J13" s="140"/>
-      <c r="K13" s="135"/>
+      <c r="I13" s="138"/>
+      <c r="J13" s="138"/>
+      <c r="K13" s="200"/>
       <c r="L13" s="51"/>
       <c r="M13" s="51" t="s">
         <v>143</v>
@@ -2442,9 +2437,9 @@
       <c r="N13" s="77"/>
     </row>
     <row r="14" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="145"/>
-      <c r="B14" s="143"/>
-      <c r="C14" s="156"/>
+      <c r="A14" s="157"/>
+      <c r="B14" s="161"/>
+      <c r="C14" s="175"/>
       <c r="D14" s="50" t="s">
         <v>108</v>
       </c>
@@ -2456,9 +2451,9 @@
       <c r="H14" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="140"/>
-      <c r="J14" s="140"/>
-      <c r="K14" s="135"/>
+      <c r="I14" s="138"/>
+      <c r="J14" s="138"/>
+      <c r="K14" s="200"/>
       <c r="L14" s="51"/>
       <c r="M14" s="51" t="s">
         <v>143</v>
@@ -2466,9 +2461,9 @@
       <c r="N14" s="77"/>
     </row>
     <row r="15" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="145"/>
-      <c r="B15" s="158"/>
-      <c r="C15" s="157"/>
+      <c r="A15" s="157"/>
+      <c r="B15" s="193"/>
+      <c r="C15" s="192"/>
       <c r="D15" s="50" t="s">
         <v>30</v>
       </c>
@@ -2484,9 +2479,9 @@
       <c r="H15" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="I15" s="141"/>
-      <c r="J15" s="141"/>
-      <c r="K15" s="136"/>
+      <c r="I15" s="139"/>
+      <c r="J15" s="139"/>
+      <c r="K15" s="201"/>
       <c r="L15" s="51"/>
       <c r="M15" s="51" t="s">
         <v>143</v>
@@ -2494,7 +2489,7 @@
       <c r="N15" s="77"/>
     </row>
     <row r="16" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="145"/>
+      <c r="A16" s="157"/>
       <c r="B16" s="75">
         <v>44439</v>
       </c>
@@ -2510,7 +2505,7 @@
         <v>150</v>
       </c>
       <c r="J16" s="127" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K16" s="48"/>
       <c r="L16" s="48"/>
@@ -2518,11 +2513,11 @@
       <c r="N16" s="77"/>
     </row>
     <row r="17" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="145"/>
-      <c r="B17" s="165">
+      <c r="A17" s="157"/>
+      <c r="B17" s="150">
         <v>44440</v>
       </c>
-      <c r="C17" s="151" t="s">
+      <c r="C17" s="165" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="55" t="s">
@@ -2535,28 +2530,28 @@
         <v>69</v>
       </c>
       <c r="G17" s="55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H17" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="191" t="s">
-        <v>172</v>
-      </c>
-      <c r="J17" s="191" t="s">
-        <v>176</v>
+      <c r="I17" s="131" t="s">
+        <v>171</v>
+      </c>
+      <c r="J17" s="131" t="s">
+        <v>175</v>
       </c>
       <c r="K17" s="95"/>
-      <c r="L17" s="191"/>
+      <c r="L17" s="131"/>
       <c r="M17" s="55" t="s">
         <v>143</v>
       </c>
       <c r="N17" s="77"/>
     </row>
     <row r="18" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="145"/>
-      <c r="B18" s="149"/>
-      <c r="C18" s="152"/>
+      <c r="A18" s="157"/>
+      <c r="B18" s="186"/>
+      <c r="C18" s="173"/>
       <c r="D18" s="55" t="s">
         <v>59</v>
       </c>
@@ -2570,21 +2565,21 @@
       <c r="H18" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="192"/>
-      <c r="J18" s="192"/>
+      <c r="I18" s="132"/>
+      <c r="J18" s="132"/>
       <c r="K18" s="96"/>
-      <c r="L18" s="192"/>
+      <c r="L18" s="132"/>
       <c r="M18" s="55" t="s">
         <v>143</v>
       </c>
       <c r="N18" s="77"/>
     </row>
     <row r="19" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="145"/>
-      <c r="B19" s="142">
+      <c r="A19" s="157"/>
+      <c r="B19" s="160">
         <v>44441</v>
       </c>
-      <c r="C19" s="153" t="s">
+      <c r="C19" s="174" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="51" t="s">
@@ -2598,41 +2593,41 @@
         <v>14</v>
       </c>
       <c r="H19" s="51"/>
-      <c r="I19" s="193" t="s">
-        <v>168</v>
-      </c>
-      <c r="J19" s="193" t="s">
-        <v>178</v>
+      <c r="I19" s="133" t="s">
+        <v>167</v>
+      </c>
+      <c r="J19" s="133" t="s">
+        <v>177</v>
       </c>
       <c r="K19" s="93"/>
-      <c r="L19" s="193"/>
+      <c r="L19" s="133"/>
       <c r="M19" s="51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N19" s="77"/>
     </row>
     <row r="20" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="145"/>
-      <c r="B20" s="147"/>
-      <c r="C20" s="154"/>
+      <c r="A20" s="157"/>
+      <c r="B20" s="162"/>
+      <c r="C20" s="176"/>
       <c r="D20" s="51"/>
       <c r="E20" s="61"/>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
       <c r="H20" s="51"/>
-      <c r="I20" s="194"/>
-      <c r="J20" s="194"/>
+      <c r="I20" s="134"/>
+      <c r="J20" s="134"/>
       <c r="K20" s="94"/>
-      <c r="L20" s="194"/>
+      <c r="L20" s="134"/>
       <c r="M20" s="51"/>
       <c r="N20" s="77"/>
     </row>
     <row r="21" spans="1:14" ht="38.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="145"/>
-      <c r="B21" s="148">
+      <c r="A21" s="157"/>
+      <c r="B21" s="190">
         <v>44442</v>
       </c>
-      <c r="C21" s="155" t="s">
+      <c r="C21" s="172" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="55" t="s">
@@ -2645,16 +2640,16 @@
         <v>78</v>
       </c>
       <c r="G21" s="55" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H21" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="I21" s="191" t="s">
-        <v>173</v>
+      <c r="I21" s="131" t="s">
+        <v>172</v>
       </c>
       <c r="J21" s="128" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K21" s="55"/>
       <c r="L21" s="55"/>
@@ -2664,9 +2659,9 @@
       <c r="N21" s="77"/>
     </row>
     <row r="22" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="146"/>
-      <c r="B22" s="149"/>
-      <c r="C22" s="152"/>
+      <c r="A22" s="189"/>
+      <c r="B22" s="186"/>
+      <c r="C22" s="173"/>
       <c r="D22" s="55" t="s">
         <v>63</v>
       </c>
@@ -2678,7 +2673,7 @@
       <c r="H22" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="192"/>
+      <c r="I22" s="132"/>
       <c r="J22" s="55"/>
       <c r="K22" s="55"/>
       <c r="L22" s="55"/>
@@ -2707,13 +2702,13 @@
       <c r="N23" s="77"/>
     </row>
     <row r="24" spans="1:14" ht="27.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="168" t="s">
+      <c r="A24" s="155" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="142">
+      <c r="B24" s="160">
         <v>44445</v>
       </c>
-      <c r="C24" s="153" t="s">
+      <c r="C24" s="174" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="53" t="s">
@@ -2731,11 +2726,11 @@
       <c r="H24" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="I24" s="193" t="s">
+      <c r="I24" s="133" t="s">
         <v>155</v>
       </c>
-      <c r="J24" s="193"/>
-      <c r="K24" s="129" t="s">
+      <c r="J24" s="133"/>
+      <c r="K24" s="194" t="s">
         <v>118</v>
       </c>
       <c r="L24" s="51"/>
@@ -2745,9 +2740,9 @@
       <c r="N24" s="77"/>
     </row>
     <row r="25" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="144"/>
-      <c r="B25" s="143"/>
-      <c r="C25" s="156"/>
+      <c r="A25" s="156"/>
+      <c r="B25" s="161"/>
+      <c r="C25" s="175"/>
       <c r="D25" s="51" t="s">
         <v>82</v>
       </c>
@@ -2761,9 +2756,9 @@
       <c r="H25" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="199"/>
-      <c r="J25" s="199"/>
-      <c r="K25" s="130"/>
+      <c r="I25" s="135"/>
+      <c r="J25" s="135"/>
+      <c r="K25" s="195"/>
       <c r="L25" s="51"/>
       <c r="M25" s="51" t="s">
         <v>103</v>
@@ -2771,9 +2766,9 @@
       <c r="N25" s="77"/>
     </row>
     <row r="26" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="144"/>
-      <c r="B26" s="143"/>
-      <c r="C26" s="156"/>
+      <c r="A26" s="156"/>
+      <c r="B26" s="161"/>
+      <c r="C26" s="175"/>
       <c r="D26" s="51" t="s">
         <v>116</v>
       </c>
@@ -2787,9 +2782,9 @@
       <c r="H26" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="199"/>
-      <c r="J26" s="199"/>
-      <c r="K26" s="130"/>
+      <c r="I26" s="135"/>
+      <c r="J26" s="135"/>
+      <c r="K26" s="195"/>
       <c r="L26" s="51"/>
       <c r="M26" s="51" t="s">
         <v>103</v>
@@ -2797,9 +2792,9 @@
       <c r="N26" s="77"/>
     </row>
     <row r="27" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="144"/>
-      <c r="B27" s="143"/>
-      <c r="C27" s="156"/>
+      <c r="A27" s="156"/>
+      <c r="B27" s="161"/>
+      <c r="C27" s="175"/>
       <c r="D27" s="51" t="s">
         <v>30</v>
       </c>
@@ -2815,9 +2810,9 @@
       <c r="H27" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="I27" s="199"/>
-      <c r="J27" s="199"/>
-      <c r="K27" s="131"/>
+      <c r="I27" s="135"/>
+      <c r="J27" s="135"/>
+      <c r="K27" s="196"/>
       <c r="L27" s="51"/>
       <c r="M27" s="51" t="s">
         <v>103</v>
@@ -2825,7 +2820,7 @@
       <c r="N27" s="77"/>
     </row>
     <row r="28" spans="1:14" s="69" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="145"/>
+      <c r="A28" s="157"/>
       <c r="B28" s="75">
         <v>44446</v>
       </c>
@@ -2846,11 +2841,11 @@
       <c r="M28" s="48"/>
     </row>
     <row r="29" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="145"/>
-      <c r="B29" s="165">
+      <c r="A29" s="157"/>
+      <c r="B29" s="150">
         <v>44447</v>
       </c>
-      <c r="C29" s="151" t="s">
+      <c r="C29" s="165" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="55" t="s">
@@ -2868,13 +2863,13 @@
       <c r="H29" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="I29" s="191" t="s">
+      <c r="I29" s="131" t="s">
         <v>102</v>
       </c>
-      <c r="J29" s="191" t="s">
+      <c r="J29" s="131" t="s">
         <v>100</v>
       </c>
-      <c r="K29" s="137" t="s">
+      <c r="K29" s="202" t="s">
         <v>125</v>
       </c>
       <c r="L29" s="55"/>
@@ -2884,9 +2879,9 @@
       <c r="N29" s="77"/>
     </row>
     <row r="30" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="145"/>
-      <c r="B30" s="183"/>
-      <c r="C30" s="169"/>
+      <c r="A30" s="157"/>
+      <c r="B30" s="151"/>
+      <c r="C30" s="166"/>
       <c r="D30" s="55" t="s">
         <v>59</v>
       </c>
@@ -2900,9 +2895,9 @@
       <c r="H30" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="192"/>
-      <c r="J30" s="192"/>
-      <c r="K30" s="138"/>
+      <c r="I30" s="132"/>
+      <c r="J30" s="132"/>
+      <c r="K30" s="203"/>
       <c r="L30" s="55"/>
       <c r="M30" s="55" t="s">
         <v>103</v>
@@ -2910,7 +2905,7 @@
       <c r="N30" s="87"/>
     </row>
     <row r="31" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="145"/>
+      <c r="A31" s="157"/>
       <c r="B31" s="88">
         <v>44448</v>
       </c>
@@ -2938,11 +2933,11 @@
       <c r="N31" s="77"/>
     </row>
     <row r="32" spans="1:14" ht="12.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="145"/>
-      <c r="B32" s="165">
+      <c r="A32" s="157"/>
+      <c r="B32" s="150">
         <v>44449</v>
       </c>
-      <c r="C32" s="155" t="s">
+      <c r="C32" s="172" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="55" t="s">
@@ -2960,19 +2955,19 @@
       <c r="H32" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="I32" s="191" t="s">
+      <c r="I32" s="131" t="s">
         <v>117</v>
       </c>
-      <c r="J32" s="191"/>
+      <c r="J32" s="131"/>
       <c r="K32" s="95"/>
       <c r="L32" s="55"/>
       <c r="M32" s="55"/>
       <c r="N32" s="77"/>
     </row>
     <row r="33" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="145"/>
-      <c r="B33" s="149"/>
-      <c r="C33" s="152"/>
+      <c r="A33" s="157"/>
+      <c r="B33" s="186"/>
+      <c r="C33" s="173"/>
       <c r="D33" s="55" t="s">
         <v>63</v>
       </c>
@@ -2986,8 +2981,8 @@
       <c r="H33" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="192"/>
-      <c r="J33" s="192"/>
+      <c r="I33" s="132"/>
+      <c r="J33" s="132"/>
       <c r="K33" s="96"/>
       <c r="L33" s="55"/>
       <c r="M33" s="55"/>
@@ -3013,13 +3008,13 @@
       <c r="N34" s="77"/>
     </row>
     <row r="35" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="168" t="s">
+      <c r="A35" s="155" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="142">
+      <c r="B35" s="160">
         <v>44452</v>
       </c>
-      <c r="C35" s="153" t="s">
+      <c r="C35" s="174" t="s">
         <v>7</v>
       </c>
       <c r="D35" s="52" t="s">
@@ -3032,18 +3027,18 @@
         <v>29</v>
       </c>
       <c r="G35" s="51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H35" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="I35" s="139" t="s">
+      <c r="I35" s="137" t="s">
         <v>79</v>
       </c>
-      <c r="J35" s="203" t="s">
+      <c r="J35" s="136" t="s">
         <v>156</v>
       </c>
-      <c r="K35" s="139" t="s">
+      <c r="K35" s="137" t="s">
         <v>126</v>
       </c>
       <c r="L35" s="51"/>
@@ -3052,9 +3047,9 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="12.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="144"/>
-      <c r="B36" s="143"/>
-      <c r="C36" s="156"/>
+      <c r="A36" s="156"/>
+      <c r="B36" s="161"/>
+      <c r="C36" s="175"/>
       <c r="D36" s="50" t="s">
         <v>63</v>
       </c>
@@ -3070,9 +3065,9 @@
       <c r="H36" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="140"/>
-      <c r="J36" s="199"/>
-      <c r="K36" s="140"/>
+      <c r="I36" s="138"/>
+      <c r="J36" s="135"/>
+      <c r="K36" s="138"/>
       <c r="L36" s="51"/>
       <c r="M36" s="51" t="s">
         <v>143</v>
@@ -3080,9 +3075,9 @@
       <c r="N36" s="77"/>
     </row>
     <row r="37" spans="1:14" ht="12.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="144"/>
-      <c r="B37" s="143"/>
-      <c r="C37" s="156"/>
+      <c r="A37" s="156"/>
+      <c r="B37" s="161"/>
+      <c r="C37" s="175"/>
       <c r="D37" s="50" t="s">
         <v>108</v>
       </c>
@@ -3098,9 +3093,9 @@
       <c r="H37" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I37" s="140"/>
-      <c r="J37" s="199"/>
-      <c r="K37" s="140"/>
+      <c r="I37" s="138"/>
+      <c r="J37" s="135"/>
+      <c r="K37" s="138"/>
       <c r="L37" s="51"/>
       <c r="M37" s="51" t="s">
         <v>143</v>
@@ -3108,9 +3103,9 @@
       <c r="N37" s="77"/>
     </row>
     <row r="38" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="144"/>
-      <c r="B38" s="147"/>
-      <c r="C38" s="154"/>
+      <c r="A38" s="156"/>
+      <c r="B38" s="162"/>
+      <c r="C38" s="176"/>
       <c r="D38" s="50" t="s">
         <v>30</v>
       </c>
@@ -3121,14 +3116,14 @@
         <v>29</v>
       </c>
       <c r="G38" s="51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H38" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="I38" s="141"/>
-      <c r="J38" s="194"/>
-      <c r="K38" s="141"/>
+      <c r="I38" s="139"/>
+      <c r="J38" s="134"/>
+      <c r="K38" s="139"/>
       <c r="L38" s="51"/>
       <c r="M38" s="51" t="s">
         <v>143</v>
@@ -3136,7 +3131,7 @@
       <c r="N38" s="77"/>
     </row>
     <row r="39" spans="1:14" s="69" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="145"/>
+      <c r="A39" s="157"/>
       <c r="B39" s="90">
         <v>44453</v>
       </c>
@@ -3156,11 +3151,11 @@
       <c r="N39" s="87"/>
     </row>
     <row r="40" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="145"/>
-      <c r="B40" s="165">
+      <c r="A40" s="157"/>
+      <c r="B40" s="150">
         <v>44454</v>
       </c>
-      <c r="C40" s="151" t="s">
+      <c r="C40" s="165" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="55" t="s">
@@ -3178,8 +3173,8 @@
       <c r="H40" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="I40" s="191"/>
-      <c r="J40" s="191"/>
+      <c r="I40" s="131"/>
+      <c r="J40" s="131"/>
       <c r="K40" s="95"/>
       <c r="L40" s="55"/>
       <c r="M40" s="55" t="s">
@@ -3187,9 +3182,9 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="145"/>
-      <c r="B41" s="183"/>
-      <c r="C41" s="169"/>
+      <c r="A41" s="157"/>
+      <c r="B41" s="151"/>
+      <c r="C41" s="166"/>
       <c r="D41" s="55" t="s">
         <v>59</v>
       </c>
@@ -3201,8 +3196,8 @@
       <c r="H41" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I41" s="192"/>
-      <c r="J41" s="192"/>
+      <c r="I41" s="132"/>
+      <c r="J41" s="132"/>
       <c r="K41" s="96"/>
       <c r="L41" s="55"/>
       <c r="M41" s="55" t="s">
@@ -3211,7 +3206,7 @@
       <c r="N41" s="77"/>
     </row>
     <row r="42" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="145"/>
+      <c r="A42" s="157"/>
       <c r="B42" s="88">
         <v>44455</v>
       </c>
@@ -3239,11 +3234,11 @@
       <c r="N42" s="77"/>
     </row>
     <row r="43" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="145"/>
-      <c r="B43" s="166">
+      <c r="A43" s="157"/>
+      <c r="B43" s="187">
         <v>44456</v>
       </c>
-      <c r="C43" s="175" t="s">
+      <c r="C43" s="177" t="s">
         <v>12</v>
       </c>
       <c r="D43" s="55" t="s">
@@ -3256,14 +3251,14 @@
         <v>76</v>
       </c>
       <c r="G43" s="55" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H43" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="I43" s="191"/>
-      <c r="J43" s="191"/>
-      <c r="K43" s="132" t="s">
+      <c r="I43" s="131"/>
+      <c r="J43" s="131"/>
+      <c r="K43" s="197" t="s">
         <v>119</v>
       </c>
       <c r="L43" s="55"/>
@@ -3273,9 +3268,9 @@
       <c r="N43" s="77"/>
     </row>
     <row r="44" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="145"/>
-      <c r="B44" s="167"/>
-      <c r="C44" s="175"/>
+      <c r="A44" s="157"/>
+      <c r="B44" s="188"/>
+      <c r="C44" s="177"/>
       <c r="D44" s="55" t="s">
         <v>63</v>
       </c>
@@ -3287,9 +3282,9 @@
       <c r="H44" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I44" s="192"/>
-      <c r="J44" s="192"/>
-      <c r="K44" s="133"/>
+      <c r="I44" s="132"/>
+      <c r="J44" s="132"/>
+      <c r="K44" s="198"/>
       <c r="L44" s="55"/>
       <c r="M44" s="55" t="s">
         <v>103</v>
@@ -3315,13 +3310,13 @@
       <c r="M45" s="47"/>
     </row>
     <row r="46" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="178" t="s">
+      <c r="A46" s="145" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="184">
+      <c r="B46" s="152">
         <v>44459</v>
       </c>
-      <c r="C46" s="176" t="s">
+      <c r="C46" s="178" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="52" t="s">
@@ -3339,8 +3334,8 @@
       <c r="H46" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="I46" s="193"/>
-      <c r="J46" s="195"/>
+      <c r="I46" s="133"/>
+      <c r="J46" s="140"/>
       <c r="K46" s="62"/>
       <c r="L46" s="50"/>
       <c r="M46" s="50" t="s">
@@ -3348,9 +3343,9 @@
       </c>
     </row>
     <row r="47" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="179"/>
-      <c r="B47" s="184"/>
-      <c r="C47" s="176"/>
+      <c r="A47" s="146"/>
+      <c r="B47" s="152"/>
+      <c r="C47" s="178"/>
       <c r="D47" s="50" t="s">
         <v>63</v>
       </c>
@@ -3362,8 +3357,8 @@
       <c r="H47" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I47" s="199"/>
-      <c r="J47" s="200"/>
+      <c r="I47" s="135"/>
+      <c r="J47" s="142"/>
       <c r="K47" s="63"/>
       <c r="L47" s="50"/>
       <c r="M47" s="50" t="s">
@@ -3371,9 +3366,9 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="179"/>
-      <c r="B48" s="184"/>
-      <c r="C48" s="176"/>
+      <c r="A48" s="146"/>
+      <c r="B48" s="152"/>
+      <c r="C48" s="178"/>
       <c r="D48" s="50" t="s">
         <v>116</v>
       </c>
@@ -3385,8 +3380,8 @@
       <c r="H48" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I48" s="199"/>
-      <c r="J48" s="200"/>
+      <c r="I48" s="135"/>
+      <c r="J48" s="142"/>
       <c r="K48" s="63"/>
       <c r="L48" s="50"/>
       <c r="M48" s="50" t="s">
@@ -3394,9 +3389,9 @@
       </c>
     </row>
     <row r="49" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="179"/>
-      <c r="B49" s="184"/>
-      <c r="C49" s="176"/>
+      <c r="A49" s="146"/>
+      <c r="B49" s="152"/>
+      <c r="C49" s="178"/>
       <c r="D49" s="50" t="s">
         <v>30</v>
       </c>
@@ -3412,8 +3407,8 @@
       <c r="H49" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="I49" s="194"/>
-      <c r="J49" s="196"/>
+      <c r="I49" s="134"/>
+      <c r="J49" s="141"/>
       <c r="K49" s="64"/>
       <c r="L49" s="50"/>
       <c r="M49" s="50" t="s">
@@ -3421,7 +3416,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" s="69" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="179"/>
+      <c r="A50" s="146"/>
       <c r="B50" s="66">
         <v>44460</v>
       </c>
@@ -3440,11 +3435,11 @@
       <c r="M50" s="47"/>
     </row>
     <row r="51" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="179"/>
-      <c r="B51" s="185">
+      <c r="A51" s="146"/>
+      <c r="B51" s="153">
         <v>44461</v>
       </c>
-      <c r="C51" s="171" t="s">
+      <c r="C51" s="168" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="54" t="s">
@@ -3462,10 +3457,10 @@
       <c r="H51" s="54" t="s">
         <v>134</v>
       </c>
-      <c r="I51" s="191" t="s">
+      <c r="I51" s="131" t="s">
         <v>101</v>
       </c>
-      <c r="J51" s="201"/>
+      <c r="J51" s="143"/>
       <c r="K51" s="98"/>
       <c r="L51" s="54"/>
       <c r="M51" s="54" t="s">
@@ -3473,9 +3468,9 @@
       </c>
     </row>
     <row r="52" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="179"/>
-      <c r="B52" s="186"/>
-      <c r="C52" s="172"/>
+      <c r="A52" s="146"/>
+      <c r="B52" s="154"/>
+      <c r="C52" s="169"/>
       <c r="D52" s="54" t="s">
         <v>59</v>
       </c>
@@ -3487,8 +3482,8 @@
       <c r="H52" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="I52" s="192"/>
-      <c r="J52" s="202"/>
+      <c r="I52" s="132"/>
+      <c r="J52" s="144"/>
       <c r="K52" s="99"/>
       <c r="L52" s="54"/>
       <c r="M52" s="54" t="s">
@@ -3496,7 +3491,7 @@
       </c>
     </row>
     <row r="53" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="179"/>
+      <c r="A53" s="146"/>
       <c r="B53" s="67">
         <v>44462</v>
       </c>
@@ -3523,11 +3518,11 @@
       </c>
     </row>
     <row r="54" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="179"/>
-      <c r="B54" s="187">
+      <c r="A54" s="146"/>
+      <c r="B54" s="158">
         <v>44463</v>
       </c>
-      <c r="C54" s="173" t="s">
+      <c r="C54" s="170" t="s">
         <v>12</v>
       </c>
       <c r="D54" s="54" t="s">
@@ -3537,16 +3532,16 @@
         <v>2</v>
       </c>
       <c r="F54" s="54" t="s">
+        <v>169</v>
+      </c>
+      <c r="G54" s="54" t="s">
         <v>170</v>
-      </c>
-      <c r="G54" s="54" t="s">
-        <v>171</v>
       </c>
       <c r="H54" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="I54" s="191"/>
-      <c r="J54" s="201"/>
+      <c r="I54" s="131"/>
+      <c r="J54" s="143"/>
       <c r="K54" s="98"/>
       <c r="L54" s="55" t="s">
         <v>107</v>
@@ -3556,9 +3551,9 @@
       </c>
     </row>
     <row r="55" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="180"/>
-      <c r="B55" s="188"/>
-      <c r="C55" s="174"/>
+      <c r="A55" s="147"/>
+      <c r="B55" s="159"/>
+      <c r="C55" s="171"/>
       <c r="D55" s="54" t="s">
         <v>63</v>
       </c>
@@ -3570,8 +3565,8 @@
       <c r="H55" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="I55" s="192"/>
-      <c r="J55" s="202"/>
+      <c r="I55" s="132"/>
+      <c r="J55" s="144"/>
       <c r="K55" s="99"/>
       <c r="L55" s="54"/>
       <c r="M55" s="54" t="s">
@@ -3597,13 +3592,13 @@
       <c r="M56" s="47"/>
     </row>
     <row r="57" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="181" t="s">
+      <c r="A57" s="148" t="s">
         <v>75</v>
       </c>
-      <c r="B57" s="189">
+      <c r="B57" s="163">
         <v>44466</v>
       </c>
-      <c r="C57" s="177" t="s">
+      <c r="C57" s="179" t="s">
         <v>7</v>
       </c>
       <c r="D57" s="50" t="s">
@@ -3621,8 +3616,8 @@
       <c r="H57" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="I57" s="195"/>
-      <c r="J57" s="195"/>
+      <c r="I57" s="140"/>
+      <c r="J57" s="140"/>
       <c r="K57" s="62"/>
       <c r="L57" s="50"/>
       <c r="M57" s="50" t="s">
@@ -3630,9 +3625,9 @@
       </c>
     </row>
     <row r="58" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="182"/>
-      <c r="B58" s="190"/>
-      <c r="C58" s="177"/>
+      <c r="A58" s="149"/>
+      <c r="B58" s="164"/>
+      <c r="C58" s="179"/>
       <c r="D58" s="50" t="s">
         <v>120</v>
       </c>
@@ -3644,8 +3639,8 @@
         <v>14</v>
       </c>
       <c r="H58" s="97"/>
-      <c r="I58" s="196"/>
-      <c r="J58" s="196"/>
+      <c r="I58" s="141"/>
+      <c r="J58" s="141"/>
       <c r="K58" s="64"/>
       <c r="L58" s="97"/>
       <c r="M58" s="97" t="s">
@@ -3653,7 +3648,7 @@
       </c>
     </row>
     <row r="59" spans="1:14" s="69" customFormat="1" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="182"/>
+      <c r="A59" s="149"/>
       <c r="B59" s="66">
         <v>44467</v>
       </c>
@@ -3675,11 +3670,11 @@
       <c r="N59" s="34"/>
     </row>
     <row r="60" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="182"/>
-      <c r="B60" s="185">
+      <c r="A60" s="149"/>
+      <c r="B60" s="153">
         <v>44468</v>
       </c>
-      <c r="C60" s="170" t="s">
+      <c r="C60" s="167" t="s">
         <v>13</v>
       </c>
       <c r="D60" s="54" t="s">
@@ -3697,31 +3692,31 @@
       <c r="H60" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="I60" s="197"/>
-      <c r="J60" s="197"/>
-      <c r="K60" s="197"/>
+      <c r="I60" s="129"/>
+      <c r="J60" s="129"/>
+      <c r="K60" s="129"/>
       <c r="L60" s="57"/>
       <c r="M60" s="57" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="182"/>
-      <c r="B61" s="186"/>
-      <c r="C61" s="170"/>
+      <c r="A61" s="149"/>
+      <c r="B61" s="154"/>
+      <c r="C61" s="167"/>
       <c r="D61" s="54"/>
       <c r="E61" s="119"/>
       <c r="F61" s="57"/>
       <c r="G61" s="57"/>
       <c r="H61" s="57"/>
-      <c r="I61" s="198"/>
-      <c r="J61" s="198"/>
-      <c r="K61" s="198"/>
+      <c r="I61" s="130"/>
+      <c r="J61" s="130"/>
+      <c r="K61" s="130"/>
       <c r="L61" s="57"/>
       <c r="M61" s="57"/>
     </row>
     <row r="62" spans="1:14" ht="12.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="182"/>
+      <c r="A62" s="149"/>
       <c r="B62" s="67">
         <v>44469</v>
       </c>
@@ -3740,7 +3735,7 @@
       <c r="M62" s="97"/>
     </row>
     <row r="63" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="182"/>
+      <c r="A63" s="149"/>
       <c r="B63" s="124">
         <v>44470</v>
       </c>
@@ -3802,15 +3797,86 @@
       <c r="M65" s="69"/>
     </row>
     <row r="66" spans="1:13" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="160" t="s">
+      <c r="A66" s="181" t="s">
         <v>92</v>
       </c>
-      <c r="B66" s="161"/>
-      <c r="C66" s="162"/>
+      <c r="B66" s="182"/>
+      <c r="C66" s="183"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M63" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="87">
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="K35:K38"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A12:A22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A24:A33"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="A46:A55"/>
+    <mergeCell ref="A57:A63"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A35:A44"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="I46:I49"/>
+    <mergeCell ref="J46:J49"/>
+    <mergeCell ref="I51:I52"/>
+    <mergeCell ref="J51:J52"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="J54:J55"/>
     <mergeCell ref="K60:K61"/>
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="L17:L18"/>
@@ -3827,77 +3893,6 @@
     <mergeCell ref="J43:J44"/>
     <mergeCell ref="I35:I38"/>
     <mergeCell ref="I40:I41"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="I57:I58"/>
-    <mergeCell ref="J57:J58"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="I46:I49"/>
-    <mergeCell ref="J46:J49"/>
-    <mergeCell ref="I51:I52"/>
-    <mergeCell ref="J51:J52"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="A46:A55"/>
-    <mergeCell ref="A57:A63"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A35:A44"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A24:A33"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="A12:A22"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="K43:K44"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="K35:K38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J35" r:id="rId1" xr:uid="{6F56A95F-302D-430F-BB93-125813A81349}"/>
@@ -3994,7 +3989,7 @@
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="212">
+      <c r="A8" s="211">
         <v>34</v>
       </c>
       <c r="B8" s="30" t="s">
@@ -4010,8 +4005,8 @@
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="212"/>
-      <c r="B9" s="206" t="s">
+      <c r="A9" s="211"/>
+      <c r="B9" s="213" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="23" t="s">
@@ -4034,8 +4029,8 @@
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="212"/>
-      <c r="B10" s="221"/>
+      <c r="A10" s="211"/>
+      <c r="B10" s="214"/>
       <c r="C10" s="23" t="s">
         <v>22</v>
       </c>
@@ -4054,8 +4049,8 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="51.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="212"/>
-      <c r="B11" s="221"/>
+      <c r="A11" s="211"/>
+      <c r="B11" s="214"/>
       <c r="C11" s="17" t="s">
         <v>35</v>
       </c>
@@ -4078,8 +4073,8 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="212"/>
-      <c r="B12" s="222"/>
+      <c r="A12" s="211"/>
+      <c r="B12" s="215"/>
       <c r="C12" s="17" t="s">
         <v>40</v>
       </c>
@@ -4098,8 +4093,8 @@
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="212"/>
-      <c r="B13" s="223" t="s">
+      <c r="A13" s="211"/>
+      <c r="B13" s="216" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="30" t="s">
@@ -4122,8 +4117,8 @@
       <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:10" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="212"/>
-      <c r="B14" s="224"/>
+      <c r="A14" s="211"/>
+      <c r="B14" s="217"/>
       <c r="C14" s="30" t="s">
         <v>22</v>
       </c>
@@ -4142,8 +4137,8 @@
       <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="212"/>
-      <c r="B15" s="225"/>
+      <c r="A15" s="211"/>
+      <c r="B15" s="218"/>
       <c r="C15" s="30" t="s">
         <v>41</v>
       </c>
@@ -4162,8 +4157,8 @@
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10" ht="52.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="212"/>
-      <c r="B16" s="206" t="s">
+      <c r="A16" s="211"/>
+      <c r="B16" s="213" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="23" t="s">
@@ -4180,8 +4175,8 @@
       <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" ht="52.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="212"/>
-      <c r="B17" s="222"/>
+      <c r="A17" s="211"/>
+      <c r="B17" s="215"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="14"/>
@@ -4196,8 +4191,8 @@
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="212"/>
-      <c r="B18" s="223" t="s">
+      <c r="A18" s="211"/>
+      <c r="B18" s="216" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="30" t="s">
@@ -4218,8 +4213,8 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="212"/>
-      <c r="B19" s="224"/>
+      <c r="A19" s="211"/>
+      <c r="B19" s="217"/>
       <c r="C19" s="30" t="s">
         <v>22</v>
       </c>
@@ -4238,8 +4233,8 @@
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="220"/>
-      <c r="B20" s="225"/>
+      <c r="A20" s="212"/>
+      <c r="B20" s="218"/>
       <c r="C20" s="30" t="s">
         <v>41</v>
       </c>
@@ -4258,10 +4253,10 @@
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="214">
+      <c r="A21" s="204">
         <v>35</v>
       </c>
-      <c r="B21" s="218" t="s">
+      <c r="B21" s="207" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="9"/>
@@ -4280,8 +4275,8 @@
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="213"/>
-      <c r="B22" s="207"/>
+      <c r="A22" s="205"/>
+      <c r="B22" s="208"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="15"/>
@@ -4294,7 +4289,7 @@
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="213"/>
+      <c r="A23" s="205"/>
       <c r="B23" s="9" t="s">
         <v>10</v>
       </c>
@@ -4308,8 +4303,8 @@
       <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="213"/>
-      <c r="B24" s="218" t="s">
+      <c r="A24" s="205"/>
+      <c r="B24" s="207" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="9"/>
@@ -4328,8 +4323,8 @@
       <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="213"/>
-      <c r="B25" s="207"/>
+      <c r="A25" s="205"/>
+      <c r="B25" s="208"/>
       <c r="C25" s="9"/>
       <c r="D25" s="15"/>
       <c r="E25" s="9"/>
@@ -4340,8 +4335,8 @@
       <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="213"/>
-      <c r="B26" s="218" t="s">
+      <c r="A26" s="205"/>
+      <c r="B26" s="207" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -4358,8 +4353,8 @@
       <c r="J26" s="11"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="213"/>
-      <c r="B27" s="207"/>
+      <c r="A27" s="205"/>
+      <c r="B27" s="208"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="15"/>
@@ -4370,8 +4365,8 @@
       <c r="J27" s="11"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="213"/>
-      <c r="B28" s="226" t="s">
+      <c r="A28" s="205"/>
+      <c r="B28" s="209" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="9"/>
@@ -4384,8 +4379,8 @@
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="217"/>
-      <c r="B29" s="227"/>
+      <c r="A29" s="206"/>
+      <c r="B29" s="210"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="21"/>
@@ -4396,10 +4391,10 @@
       <c r="J29" s="11"/>
     </row>
     <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="211">
+      <c r="A30" s="224">
         <v>36</v>
       </c>
-      <c r="B30" s="206" t="s">
+      <c r="B30" s="213" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="23"/>
@@ -4418,8 +4413,8 @@
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="212"/>
-      <c r="B31" s="207"/>
+      <c r="A31" s="211"/>
+      <c r="B31" s="208"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
       <c r="E31" s="14"/>
@@ -4430,7 +4425,7 @@
       <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="213"/>
+      <c r="A32" s="205"/>
       <c r="B32" s="23" t="s">
         <v>10</v>
       </c>
@@ -4444,7 +4439,7 @@
       <c r="J32" s="11"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="213"/>
+      <c r="A33" s="205"/>
       <c r="B33" s="23" t="s">
         <v>13</v>
       </c>
@@ -4462,8 +4457,8 @@
       <c r="J33" s="11"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="213"/>
-      <c r="B34" s="206" t="s">
+      <c r="A34" s="205"/>
+      <c r="B34" s="213" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="23" t="s">
@@ -4480,8 +4475,8 @@
       <c r="J34" s="11"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="213"/>
-      <c r="B35" s="207"/>
+      <c r="A35" s="205"/>
+      <c r="B35" s="208"/>
       <c r="C35" s="23"/>
       <c r="D35" s="23"/>
       <c r="E35" s="14"/>
@@ -4492,8 +4487,8 @@
       <c r="J35" s="11"/>
     </row>
     <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="213"/>
-      <c r="B36" s="206" t="s">
+      <c r="A36" s="205"/>
+      <c r="B36" s="213" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="23"/>
@@ -4512,8 +4507,8 @@
       <c r="J36" s="11"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="213"/>
-      <c r="B37" s="207"/>
+      <c r="A37" s="205"/>
+      <c r="B37" s="208"/>
       <c r="C37" s="23"/>
       <c r="D37" s="23"/>
       <c r="E37" s="23"/>
@@ -4524,10 +4519,10 @@
       <c r="J37" s="11"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="214">
+      <c r="A38" s="204">
         <v>37</v>
       </c>
-      <c r="B38" s="218" t="s">
+      <c r="B38" s="207" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="9"/>
@@ -4540,8 +4535,8 @@
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="215"/>
-      <c r="B39" s="207"/>
+      <c r="A39" s="225"/>
+      <c r="B39" s="208"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="15"/>
@@ -4552,7 +4547,7 @@
       <c r="J39" s="11"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="216"/>
+      <c r="A40" s="226"/>
       <c r="B40" s="10" t="s">
         <v>10</v>
       </c>
@@ -4566,7 +4561,7 @@
       <c r="J40" s="11"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="216"/>
+      <c r="A41" s="226"/>
       <c r="B41" s="10" t="s">
         <v>13</v>
       </c>
@@ -4580,8 +4575,8 @@
       <c r="J41" s="11"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="216"/>
-      <c r="B42" s="218" t="s">
+      <c r="A42" s="226"/>
+      <c r="B42" s="207" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="9" t="s">
@@ -4598,8 +4593,8 @@
       <c r="J42" s="11"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="216"/>
-      <c r="B43" s="219"/>
+      <c r="A43" s="226"/>
+      <c r="B43" s="227"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -4610,8 +4605,8 @@
       <c r="J43" s="11"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="216"/>
-      <c r="B44" s="207"/>
+      <c r="A44" s="226"/>
+      <c r="B44" s="208"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="20"/>
@@ -4622,8 +4617,8 @@
       <c r="J44" s="11"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="216"/>
-      <c r="B45" s="218" t="s">
+      <c r="A45" s="226"/>
+      <c r="B45" s="207" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="9"/>
@@ -4636,8 +4631,8 @@
       <c r="J45" s="11"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="213"/>
-      <c r="B46" s="219"/>
+      <c r="A46" s="205"/>
+      <c r="B46" s="227"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -4648,8 +4643,8 @@
       <c r="J46" s="11"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="217"/>
-      <c r="B47" s="207"/>
+      <c r="A47" s="206"/>
+      <c r="B47" s="208"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="20"/>
@@ -4660,10 +4655,10 @@
       <c r="J47" s="11"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="204">
+      <c r="A48" s="219">
         <v>38</v>
       </c>
-      <c r="B48" s="206" t="s">
+      <c r="B48" s="213" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="23"/>
@@ -4676,8 +4671,8 @@
       <c r="J48" s="11"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="204"/>
-      <c r="B49" s="207"/>
+      <c r="A49" s="219"/>
+      <c r="B49" s="208"/>
       <c r="C49" s="23"/>
       <c r="D49" s="23"/>
       <c r="E49" s="23"/>
@@ -4688,7 +4683,7 @@
       <c r="J49" s="11"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="205"/>
+      <c r="A50" s="220"/>
       <c r="B50" s="23" t="s">
         <v>10</v>
       </c>
@@ -4702,7 +4697,7 @@
       <c r="J50" s="11"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="205"/>
+      <c r="A51" s="220"/>
       <c r="B51" s="23" t="s">
         <v>13</v>
       </c>
@@ -4716,7 +4711,7 @@
       <c r="J51" s="11"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="205"/>
+      <c r="A52" s="220"/>
       <c r="B52" s="23" t="s">
         <v>11</v>
       </c>
@@ -4734,8 +4729,8 @@
       <c r="J52" s="11"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="205"/>
-      <c r="B53" s="204" t="s">
+      <c r="A53" s="220"/>
+      <c r="B53" s="219" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="17"/>
@@ -4748,8 +4743,8 @@
       <c r="J53" s="11"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="205"/>
-      <c r="B54" s="205"/>
+      <c r="A54" s="220"/>
+      <c r="B54" s="220"/>
       <c r="C54" s="23"/>
       <c r="D54" s="23"/>
       <c r="E54" s="22"/>
@@ -4760,7 +4755,7 @@
       <c r="J54" s="11"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="208">
+      <c r="A55" s="221">
         <v>39</v>
       </c>
       <c r="B55" s="24" t="s">
@@ -4776,7 +4771,7 @@
       <c r="J55" s="11"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="209"/>
+      <c r="A56" s="222"/>
       <c r="B56" s="25" t="s">
         <v>10</v>
       </c>
@@ -4789,7 +4784,7 @@
       <c r="I56" s="28"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="209"/>
+      <c r="A57" s="222"/>
       <c r="B57" s="25" t="s">
         <v>13</v>
       </c>
@@ -4802,7 +4797,7 @@
       <c r="I57" s="28"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="209"/>
+      <c r="A58" s="222"/>
       <c r="B58" s="25" t="s">
         <v>11</v>
       </c>
@@ -4819,7 +4814,7 @@
       <c r="I58" s="28"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="210"/>
+      <c r="A59" s="223"/>
       <c r="B59" s="26" t="s">
         <v>12</v>
       </c>
@@ -4833,16 +4828,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A8:A20"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B20"/>
     <mergeCell ref="A48:A54"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B53:B54"/>
@@ -4855,6 +4840,16 @@
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
+    <mergeCell ref="A8:A20"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates for week 2
</commit_message>
<xml_diff>
--- a/01_studieplan_och_schema.xlsx
+++ b/01_studieplan_och_schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsabellaGagner\Documents\Programming-projects\EC\ec-python-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5B7D25-B9D4-4D8F-82E9-D0A59314D2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E61ECA2-E2A8-4564-A153-906598A6EB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="4320" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema - Python" sheetId="1" r:id="rId1"/>
@@ -537,9 +537,6 @@
     <t>Öppna och läsa från filer, spara till filer, plotting, numpy</t>
   </si>
   <si>
-    <t>pathlib, filhantering, flytta filer med shutil, f-strings</t>
-  </si>
-  <si>
     <t>Isabella, Alex</t>
   </si>
   <si>
@@ -579,7 +576,10 @@
     <t>https://realpython.com/python-f-strings/#f-strings-a-new-and-improved-way-to-format-strings-in-python</t>
   </si>
   <si>
-    <t>Repetition vecka 1, terminalkommandon, argparse, att skapa ett git-repo</t>
+    <t>Repetition vecka 1, terminalkommandon, argparse, att skapa ett git-repo, introduktion till inlämning 1</t>
+  </si>
+  <si>
+    <t>pathlib, filhantering, flytta filer med shutil</t>
   </si>
 </sst>
 </file>
@@ -1350,280 +1350,241 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1634,13 +1595,52 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2016,8 +2016,8 @@
   <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -2082,7 +2082,7 @@
       <c r="N1" s="74"/>
     </row>
     <row r="2" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="156" t="s">
+      <c r="A2" s="144" t="s">
         <v>70</v>
       </c>
       <c r="B2" s="75">
@@ -2104,11 +2104,11 @@
       <c r="N2" s="77"/>
     </row>
     <row r="3" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="156"/>
-      <c r="B3" s="185">
+      <c r="A3" s="144"/>
+      <c r="B3" s="164">
         <v>44432</v>
       </c>
-      <c r="C3" s="184" t="s">
+      <c r="C3" s="163" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="51" t="s">
@@ -2126,10 +2126,10 @@
       <c r="H3" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="184" t="s">
+      <c r="I3" s="163" t="s">
         <v>160</v>
       </c>
-      <c r="J3" s="184" t="s">
+      <c r="J3" s="163" t="s">
         <v>46</v>
       </c>
       <c r="K3" s="79"/>
@@ -2142,9 +2142,9 @@
       <c r="N3" s="77"/>
     </row>
     <row r="4" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="156"/>
-      <c r="B4" s="185"/>
-      <c r="C4" s="184"/>
+      <c r="A4" s="144"/>
+      <c r="B4" s="164"/>
+      <c r="C4" s="163"/>
       <c r="D4" s="51" t="s">
         <v>22</v>
       </c>
@@ -2160,8 +2160,8 @@
       <c r="H4" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="184"/>
-      <c r="J4" s="184"/>
+      <c r="I4" s="163"/>
+      <c r="J4" s="163"/>
       <c r="K4" s="79"/>
       <c r="L4" s="51"/>
       <c r="M4" s="51" t="s">
@@ -2170,9 +2170,9 @@
       <c r="N4" s="77"/>
     </row>
     <row r="5" spans="1:14" ht="27.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="156"/>
-      <c r="B5" s="185"/>
-      <c r="C5" s="184"/>
+      <c r="A5" s="144"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="163"/>
       <c r="D5" s="51" t="s">
         <v>58</v>
       </c>
@@ -2188,8 +2188,8 @@
       <c r="H5" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="184"/>
-      <c r="J5" s="184"/>
+      <c r="I5" s="163"/>
+      <c r="J5" s="163"/>
       <c r="K5" s="79"/>
       <c r="L5" s="51" t="s">
         <v>38</v>
@@ -2200,11 +2200,11 @@
       <c r="N5" s="77"/>
     </row>
     <row r="6" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="156"/>
-      <c r="B6" s="187">
+      <c r="A6" s="144"/>
+      <c r="B6" s="166">
         <v>44433</v>
       </c>
-      <c r="C6" s="191" t="s">
+      <c r="C6" s="150" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="55" t="s">
@@ -2222,10 +2222,10 @@
       <c r="H6" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="180" t="s">
+      <c r="I6" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="J6" s="180" t="s">
+      <c r="J6" s="159" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="56"/>
@@ -2236,9 +2236,9 @@
       <c r="N6" s="77"/>
     </row>
     <row r="7" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="156"/>
-      <c r="B7" s="187"/>
-      <c r="C7" s="191"/>
+      <c r="A7" s="144"/>
+      <c r="B7" s="166"/>
+      <c r="C7" s="150"/>
       <c r="D7" s="55" t="s">
         <v>59</v>
       </c>
@@ -2250,8 +2250,8 @@
       <c r="H7" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="180"/>
-      <c r="J7" s="180"/>
+      <c r="I7" s="159"/>
+      <c r="J7" s="159"/>
       <c r="K7" s="56"/>
       <c r="L7" s="55"/>
       <c r="M7" s="55" t="s">
@@ -2260,7 +2260,7 @@
       <c r="N7" s="77"/>
     </row>
     <row r="8" spans="1:14" ht="25.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="156"/>
+      <c r="A8" s="144"/>
       <c r="B8" s="78">
         <v>44434</v>
       </c>
@@ -2292,11 +2292,11 @@
       <c r="N8" s="77"/>
     </row>
     <row r="9" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="156"/>
-      <c r="B9" s="187">
+      <c r="A9" s="144"/>
+      <c r="B9" s="166">
         <v>44435</v>
       </c>
-      <c r="C9" s="191" t="s">
+      <c r="C9" s="150" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="55" t="s">
@@ -2314,14 +2314,14 @@
       <c r="H9" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="180" t="s">
+      <c r="I9" s="159" t="s">
         <v>151</v>
       </c>
-      <c r="J9" s="180" t="s">
+      <c r="J9" s="159" t="s">
         <v>146</v>
       </c>
       <c r="K9" s="56"/>
-      <c r="L9" s="131" t="s">
+      <c r="L9" s="191" t="s">
         <v>152</v>
       </c>
       <c r="M9" s="55" t="s">
@@ -2330,9 +2330,9 @@
       <c r="N9" s="77"/>
     </row>
     <row r="10" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="156"/>
-      <c r="B10" s="187"/>
-      <c r="C10" s="191"/>
+      <c r="A10" s="144"/>
+      <c r="B10" s="166"/>
+      <c r="C10" s="150"/>
       <c r="D10" s="55" t="s">
         <v>63</v>
       </c>
@@ -2344,10 +2344,10 @@
       <c r="H10" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="180"/>
-      <c r="J10" s="180"/>
+      <c r="I10" s="159"/>
+      <c r="J10" s="159"/>
       <c r="K10" s="56"/>
-      <c r="L10" s="132"/>
+      <c r="L10" s="192"/>
       <c r="M10" s="55" t="s">
         <v>143</v>
       </c>
@@ -2373,13 +2373,13 @@
       <c r="N11" s="77"/>
     </row>
     <row r="12" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="156" t="s">
+      <c r="A12" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="160">
+      <c r="B12" s="142">
         <v>44438</v>
       </c>
-      <c r="C12" s="174" t="s">
+      <c r="C12" s="153" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="52" t="s">
@@ -2392,18 +2392,18 @@
         <v>28</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H12" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="I12" s="137" t="s">
+      <c r="I12" s="139" t="s">
         <v>162</v>
       </c>
-      <c r="J12" s="137" t="s">
+      <c r="J12" s="139" t="s">
         <v>163</v>
       </c>
-      <c r="K12" s="199" t="s">
+      <c r="K12" s="134" t="s">
         <v>124</v>
       </c>
       <c r="L12" s="53"/>
@@ -2413,9 +2413,9 @@
       <c r="N12" s="77"/>
     </row>
     <row r="13" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="157"/>
-      <c r="B13" s="161"/>
-      <c r="C13" s="175"/>
+      <c r="A13" s="145"/>
+      <c r="B13" s="143"/>
+      <c r="C13" s="156"/>
       <c r="D13" s="50" t="s">
         <v>63</v>
       </c>
@@ -2427,9 +2427,9 @@
       <c r="H13" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="138"/>
-      <c r="J13" s="138"/>
-      <c r="K13" s="200"/>
+      <c r="I13" s="140"/>
+      <c r="J13" s="140"/>
+      <c r="K13" s="135"/>
       <c r="L13" s="51"/>
       <c r="M13" s="51" t="s">
         <v>143</v>
@@ -2437,9 +2437,9 @@
       <c r="N13" s="77"/>
     </row>
     <row r="14" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="157"/>
-      <c r="B14" s="161"/>
-      <c r="C14" s="175"/>
+      <c r="A14" s="145"/>
+      <c r="B14" s="143"/>
+      <c r="C14" s="156"/>
       <c r="D14" s="50" t="s">
         <v>108</v>
       </c>
@@ -2451,9 +2451,9 @@
       <c r="H14" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="138"/>
-      <c r="J14" s="138"/>
-      <c r="K14" s="200"/>
+      <c r="I14" s="140"/>
+      <c r="J14" s="140"/>
+      <c r="K14" s="135"/>
       <c r="L14" s="51"/>
       <c r="M14" s="51" t="s">
         <v>143</v>
@@ -2461,9 +2461,9 @@
       <c r="N14" s="77"/>
     </row>
     <row r="15" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="157"/>
-      <c r="B15" s="193"/>
-      <c r="C15" s="192"/>
+      <c r="A15" s="145"/>
+      <c r="B15" s="158"/>
+      <c r="C15" s="157"/>
       <c r="D15" s="50" t="s">
         <v>30</v>
       </c>
@@ -2479,9 +2479,9 @@
       <c r="H15" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="I15" s="139"/>
-      <c r="J15" s="139"/>
-      <c r="K15" s="201"/>
+      <c r="I15" s="141"/>
+      <c r="J15" s="141"/>
+      <c r="K15" s="136"/>
       <c r="L15" s="51"/>
       <c r="M15" s="51" t="s">
         <v>143</v>
@@ -2489,7 +2489,7 @@
       <c r="N15" s="77"/>
     </row>
     <row r="16" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="157"/>
+      <c r="A16" s="145"/>
       <c r="B16" s="75">
         <v>44439</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>150</v>
       </c>
       <c r="J16" s="127" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K16" s="48"/>
       <c r="L16" s="48"/>
@@ -2513,11 +2513,11 @@
       <c r="N16" s="77"/>
     </row>
     <row r="17" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="157"/>
-      <c r="B17" s="150">
+      <c r="A17" s="145"/>
+      <c r="B17" s="165">
         <v>44440</v>
       </c>
-      <c r="C17" s="165" t="s">
+      <c r="C17" s="151" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="55" t="s">
@@ -2535,23 +2535,23 @@
       <c r="H17" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="131" t="s">
-        <v>171</v>
-      </c>
-      <c r="J17" s="131" t="s">
-        <v>175</v>
+      <c r="I17" s="191" t="s">
+        <v>170</v>
+      </c>
+      <c r="J17" s="191" t="s">
+        <v>174</v>
       </c>
       <c r="K17" s="95"/>
-      <c r="L17" s="131"/>
+      <c r="L17" s="191"/>
       <c r="M17" s="55" t="s">
         <v>143</v>
       </c>
       <c r="N17" s="77"/>
     </row>
     <row r="18" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="157"/>
-      <c r="B18" s="186"/>
-      <c r="C18" s="173"/>
+      <c r="A18" s="145"/>
+      <c r="B18" s="149"/>
+      <c r="C18" s="152"/>
       <c r="D18" s="55" t="s">
         <v>59</v>
       </c>
@@ -2565,21 +2565,21 @@
       <c r="H18" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="132"/>
-      <c r="J18" s="132"/>
+      <c r="I18" s="192"/>
+      <c r="J18" s="192"/>
       <c r="K18" s="96"/>
-      <c r="L18" s="132"/>
+      <c r="L18" s="192"/>
       <c r="M18" s="55" t="s">
         <v>143</v>
       </c>
       <c r="N18" s="77"/>
     </row>
     <row r="19" spans="1:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="157"/>
-      <c r="B19" s="160">
+      <c r="A19" s="145"/>
+      <c r="B19" s="142">
         <v>44441</v>
       </c>
-      <c r="C19" s="174" t="s">
+      <c r="C19" s="153" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="51" t="s">
@@ -2593,41 +2593,41 @@
         <v>14</v>
       </c>
       <c r="H19" s="51"/>
-      <c r="I19" s="133" t="s">
-        <v>167</v>
-      </c>
-      <c r="J19" s="133" t="s">
-        <v>177</v>
+      <c r="I19" s="193" t="s">
+        <v>166</v>
+      </c>
+      <c r="J19" s="193" t="s">
+        <v>176</v>
       </c>
       <c r="K19" s="93"/>
-      <c r="L19" s="133"/>
+      <c r="L19" s="193"/>
       <c r="M19" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="N19" s="77"/>
     </row>
     <row r="20" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="157"/>
-      <c r="B20" s="162"/>
-      <c r="C20" s="176"/>
+      <c r="A20" s="145"/>
+      <c r="B20" s="147"/>
+      <c r="C20" s="154"/>
       <c r="D20" s="51"/>
       <c r="E20" s="61"/>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
       <c r="H20" s="51"/>
-      <c r="I20" s="134"/>
-      <c r="J20" s="134"/>
+      <c r="I20" s="194"/>
+      <c r="J20" s="194"/>
       <c r="K20" s="94"/>
-      <c r="L20" s="134"/>
+      <c r="L20" s="194"/>
       <c r="M20" s="51"/>
       <c r="N20" s="77"/>
     </row>
     <row r="21" spans="1:14" ht="38.85" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="157"/>
-      <c r="B21" s="190">
+      <c r="A21" s="145"/>
+      <c r="B21" s="148">
         <v>44442</v>
       </c>
-      <c r="C21" s="172" t="s">
+      <c r="C21" s="155" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="55" t="s">
@@ -2640,16 +2640,16 @@
         <v>78</v>
       </c>
       <c r="G21" s="55" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="H21" s="55" t="s">
         <v>129</v>
       </c>
-      <c r="I21" s="131" t="s">
-        <v>172</v>
+      <c r="I21" s="191" t="s">
+        <v>171</v>
       </c>
       <c r="J21" s="128" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K21" s="55"/>
       <c r="L21" s="55"/>
@@ -2659,9 +2659,9 @@
       <c r="N21" s="77"/>
     </row>
     <row r="22" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="189"/>
-      <c r="B22" s="186"/>
-      <c r="C22" s="173"/>
+      <c r="A22" s="146"/>
+      <c r="B22" s="149"/>
+      <c r="C22" s="152"/>
       <c r="D22" s="55" t="s">
         <v>63</v>
       </c>
@@ -2673,7 +2673,7 @@
       <c r="H22" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="132"/>
+      <c r="I22" s="192"/>
       <c r="J22" s="55"/>
       <c r="K22" s="55"/>
       <c r="L22" s="55"/>
@@ -2702,13 +2702,13 @@
       <c r="N23" s="77"/>
     </row>
     <row r="24" spans="1:14" ht="27.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="155" t="s">
+      <c r="A24" s="168" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="160">
+      <c r="B24" s="142">
         <v>44445</v>
       </c>
-      <c r="C24" s="174" t="s">
+      <c r="C24" s="153" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="53" t="s">
@@ -2726,11 +2726,11 @@
       <c r="H24" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="I24" s="133" t="s">
+      <c r="I24" s="193" t="s">
         <v>155</v>
       </c>
-      <c r="J24" s="133"/>
-      <c r="K24" s="194" t="s">
+      <c r="J24" s="193"/>
+      <c r="K24" s="129" t="s">
         <v>118</v>
       </c>
       <c r="L24" s="51"/>
@@ -2740,9 +2740,9 @@
       <c r="N24" s="77"/>
     </row>
     <row r="25" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="156"/>
-      <c r="B25" s="161"/>
-      <c r="C25" s="175"/>
+      <c r="A25" s="144"/>
+      <c r="B25" s="143"/>
+      <c r="C25" s="156"/>
       <c r="D25" s="51" t="s">
         <v>82</v>
       </c>
@@ -2756,9 +2756,9 @@
       <c r="H25" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="135"/>
-      <c r="J25" s="135"/>
-      <c r="K25" s="195"/>
+      <c r="I25" s="199"/>
+      <c r="J25" s="199"/>
+      <c r="K25" s="130"/>
       <c r="L25" s="51"/>
       <c r="M25" s="51" t="s">
         <v>103</v>
@@ -2766,9 +2766,9 @@
       <c r="N25" s="77"/>
     </row>
     <row r="26" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="156"/>
-      <c r="B26" s="161"/>
-      <c r="C26" s="175"/>
+      <c r="A26" s="144"/>
+      <c r="B26" s="143"/>
+      <c r="C26" s="156"/>
       <c r="D26" s="51" t="s">
         <v>116</v>
       </c>
@@ -2782,9 +2782,9 @@
       <c r="H26" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="135"/>
-      <c r="J26" s="135"/>
-      <c r="K26" s="195"/>
+      <c r="I26" s="199"/>
+      <c r="J26" s="199"/>
+      <c r="K26" s="130"/>
       <c r="L26" s="51"/>
       <c r="M26" s="51" t="s">
         <v>103</v>
@@ -2792,9 +2792,9 @@
       <c r="N26" s="77"/>
     </row>
     <row r="27" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="156"/>
-      <c r="B27" s="161"/>
-      <c r="C27" s="175"/>
+      <c r="A27" s="144"/>
+      <c r="B27" s="143"/>
+      <c r="C27" s="156"/>
       <c r="D27" s="51" t="s">
         <v>30</v>
       </c>
@@ -2810,9 +2810,9 @@
       <c r="H27" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="I27" s="135"/>
-      <c r="J27" s="135"/>
-      <c r="K27" s="196"/>
+      <c r="I27" s="199"/>
+      <c r="J27" s="199"/>
+      <c r="K27" s="131"/>
       <c r="L27" s="51"/>
       <c r="M27" s="51" t="s">
         <v>103</v>
@@ -2820,7 +2820,7 @@
       <c r="N27" s="77"/>
     </row>
     <row r="28" spans="1:14" s="69" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="157"/>
+      <c r="A28" s="145"/>
       <c r="B28" s="75">
         <v>44446</v>
       </c>
@@ -2841,11 +2841,11 @@
       <c r="M28" s="48"/>
     </row>
     <row r="29" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="157"/>
-      <c r="B29" s="150">
+      <c r="A29" s="145"/>
+      <c r="B29" s="165">
         <v>44447</v>
       </c>
-      <c r="C29" s="165" t="s">
+      <c r="C29" s="151" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="55" t="s">
@@ -2863,13 +2863,13 @@
       <c r="H29" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="I29" s="131" t="s">
+      <c r="I29" s="191" t="s">
         <v>102</v>
       </c>
-      <c r="J29" s="131" t="s">
+      <c r="J29" s="191" t="s">
         <v>100</v>
       </c>
-      <c r="K29" s="202" t="s">
+      <c r="K29" s="137" t="s">
         <v>125</v>
       </c>
       <c r="L29" s="55"/>
@@ -2879,9 +2879,9 @@
       <c r="N29" s="77"/>
     </row>
     <row r="30" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="157"/>
-      <c r="B30" s="151"/>
-      <c r="C30" s="166"/>
+      <c r="A30" s="145"/>
+      <c r="B30" s="183"/>
+      <c r="C30" s="169"/>
       <c r="D30" s="55" t="s">
         <v>59</v>
       </c>
@@ -2895,9 +2895,9 @@
       <c r="H30" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="132"/>
-      <c r="J30" s="132"/>
-      <c r="K30" s="203"/>
+      <c r="I30" s="192"/>
+      <c r="J30" s="192"/>
+      <c r="K30" s="138"/>
       <c r="L30" s="55"/>
       <c r="M30" s="55" t="s">
         <v>103</v>
@@ -2905,7 +2905,7 @@
       <c r="N30" s="87"/>
     </row>
     <row r="31" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="157"/>
+      <c r="A31" s="145"/>
       <c r="B31" s="88">
         <v>44448</v>
       </c>
@@ -2933,11 +2933,11 @@
       <c r="N31" s="77"/>
     </row>
     <row r="32" spans="1:14" ht="12.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="157"/>
-      <c r="B32" s="150">
+      <c r="A32" s="145"/>
+      <c r="B32" s="165">
         <v>44449</v>
       </c>
-      <c r="C32" s="172" t="s">
+      <c r="C32" s="155" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="55" t="s">
@@ -2955,19 +2955,19 @@
       <c r="H32" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="I32" s="131" t="s">
+      <c r="I32" s="191" t="s">
         <v>117</v>
       </c>
-      <c r="J32" s="131"/>
+      <c r="J32" s="191"/>
       <c r="K32" s="95"/>
       <c r="L32" s="55"/>
       <c r="M32" s="55"/>
       <c r="N32" s="77"/>
     </row>
     <row r="33" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="157"/>
-      <c r="B33" s="186"/>
-      <c r="C33" s="173"/>
+      <c r="A33" s="145"/>
+      <c r="B33" s="149"/>
+      <c r="C33" s="152"/>
       <c r="D33" s="55" t="s">
         <v>63</v>
       </c>
@@ -2981,8 +2981,8 @@
       <c r="H33" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="132"/>
-      <c r="J33" s="132"/>
+      <c r="I33" s="192"/>
+      <c r="J33" s="192"/>
       <c r="K33" s="96"/>
       <c r="L33" s="55"/>
       <c r="M33" s="55"/>
@@ -3008,13 +3008,13 @@
       <c r="N34" s="77"/>
     </row>
     <row r="35" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="155" t="s">
+      <c r="A35" s="168" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="160">
+      <c r="B35" s="142">
         <v>44452</v>
       </c>
-      <c r="C35" s="174" t="s">
+      <c r="C35" s="153" t="s">
         <v>7</v>
       </c>
       <c r="D35" s="52" t="s">
@@ -3027,18 +3027,18 @@
         <v>29</v>
       </c>
       <c r="G35" s="51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H35" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="I35" s="137" t="s">
+      <c r="I35" s="139" t="s">
         <v>79</v>
       </c>
-      <c r="J35" s="136" t="s">
+      <c r="J35" s="203" t="s">
         <v>156</v>
       </c>
-      <c r="K35" s="137" t="s">
+      <c r="K35" s="139" t="s">
         <v>126</v>
       </c>
       <c r="L35" s="51"/>
@@ -3047,9 +3047,9 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="12.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="156"/>
-      <c r="B36" s="161"/>
-      <c r="C36" s="175"/>
+      <c r="A36" s="144"/>
+      <c r="B36" s="143"/>
+      <c r="C36" s="156"/>
       <c r="D36" s="50" t="s">
         <v>63</v>
       </c>
@@ -3065,9 +3065,9 @@
       <c r="H36" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="138"/>
-      <c r="J36" s="135"/>
-      <c r="K36" s="138"/>
+      <c r="I36" s="140"/>
+      <c r="J36" s="199"/>
+      <c r="K36" s="140"/>
       <c r="L36" s="51"/>
       <c r="M36" s="51" t="s">
         <v>143</v>
@@ -3075,9 +3075,9 @@
       <c r="N36" s="77"/>
     </row>
     <row r="37" spans="1:14" ht="12.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="156"/>
-      <c r="B37" s="161"/>
-      <c r="C37" s="175"/>
+      <c r="A37" s="144"/>
+      <c r="B37" s="143"/>
+      <c r="C37" s="156"/>
       <c r="D37" s="50" t="s">
         <v>108</v>
       </c>
@@ -3093,9 +3093,9 @@
       <c r="H37" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I37" s="138"/>
-      <c r="J37" s="135"/>
-      <c r="K37" s="138"/>
+      <c r="I37" s="140"/>
+      <c r="J37" s="199"/>
+      <c r="K37" s="140"/>
       <c r="L37" s="51"/>
       <c r="M37" s="51" t="s">
         <v>143</v>
@@ -3103,9 +3103,9 @@
       <c r="N37" s="77"/>
     </row>
     <row r="38" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="156"/>
-      <c r="B38" s="162"/>
-      <c r="C38" s="176"/>
+      <c r="A38" s="144"/>
+      <c r="B38" s="147"/>
+      <c r="C38" s="154"/>
       <c r="D38" s="50" t="s">
         <v>30</v>
       </c>
@@ -3116,14 +3116,14 @@
         <v>29</v>
       </c>
       <c r="G38" s="51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H38" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="I38" s="139"/>
-      <c r="J38" s="134"/>
-      <c r="K38" s="139"/>
+      <c r="I38" s="141"/>
+      <c r="J38" s="194"/>
+      <c r="K38" s="141"/>
       <c r="L38" s="51"/>
       <c r="M38" s="51" t="s">
         <v>143</v>
@@ -3131,7 +3131,7 @@
       <c r="N38" s="77"/>
     </row>
     <row r="39" spans="1:14" s="69" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="157"/>
+      <c r="A39" s="145"/>
       <c r="B39" s="90">
         <v>44453</v>
       </c>
@@ -3151,11 +3151,11 @@
       <c r="N39" s="87"/>
     </row>
     <row r="40" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="157"/>
-      <c r="B40" s="150">
+      <c r="A40" s="145"/>
+      <c r="B40" s="165">
         <v>44454</v>
       </c>
-      <c r="C40" s="165" t="s">
+      <c r="C40" s="151" t="s">
         <v>13</v>
       </c>
       <c r="D40" s="55" t="s">
@@ -3173,8 +3173,8 @@
       <c r="H40" s="55" t="s">
         <v>131</v>
       </c>
-      <c r="I40" s="131"/>
-      <c r="J40" s="131"/>
+      <c r="I40" s="191"/>
+      <c r="J40" s="191"/>
       <c r="K40" s="95"/>
       <c r="L40" s="55"/>
       <c r="M40" s="55" t="s">
@@ -3182,9 +3182,9 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="157"/>
-      <c r="B41" s="151"/>
-      <c r="C41" s="166"/>
+      <c r="A41" s="145"/>
+      <c r="B41" s="183"/>
+      <c r="C41" s="169"/>
       <c r="D41" s="55" t="s">
         <v>59</v>
       </c>
@@ -3196,8 +3196,8 @@
       <c r="H41" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I41" s="132"/>
-      <c r="J41" s="132"/>
+      <c r="I41" s="192"/>
+      <c r="J41" s="192"/>
       <c r="K41" s="96"/>
       <c r="L41" s="55"/>
       <c r="M41" s="55" t="s">
@@ -3206,7 +3206,7 @@
       <c r="N41" s="77"/>
     </row>
     <row r="42" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="157"/>
+      <c r="A42" s="145"/>
       <c r="B42" s="88">
         <v>44455</v>
       </c>
@@ -3234,11 +3234,11 @@
       <c r="N42" s="77"/>
     </row>
     <row r="43" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="157"/>
-      <c r="B43" s="187">
+      <c r="A43" s="145"/>
+      <c r="B43" s="166">
         <v>44456</v>
       </c>
-      <c r="C43" s="177" t="s">
+      <c r="C43" s="175" t="s">
         <v>12</v>
       </c>
       <c r="D43" s="55" t="s">
@@ -3251,14 +3251,14 @@
         <v>76</v>
       </c>
       <c r="G43" s="55" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H43" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="I43" s="131"/>
-      <c r="J43" s="131"/>
-      <c r="K43" s="197" t="s">
+      <c r="I43" s="191"/>
+      <c r="J43" s="191"/>
+      <c r="K43" s="132" t="s">
         <v>119</v>
       </c>
       <c r="L43" s="55"/>
@@ -3268,9 +3268,9 @@
       <c r="N43" s="77"/>
     </row>
     <row r="44" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="157"/>
-      <c r="B44" s="188"/>
-      <c r="C44" s="177"/>
+      <c r="A44" s="145"/>
+      <c r="B44" s="167"/>
+      <c r="C44" s="175"/>
       <c r="D44" s="55" t="s">
         <v>63</v>
       </c>
@@ -3282,9 +3282,9 @@
       <c r="H44" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="I44" s="132"/>
-      <c r="J44" s="132"/>
-      <c r="K44" s="198"/>
+      <c r="I44" s="192"/>
+      <c r="J44" s="192"/>
+      <c r="K44" s="133"/>
       <c r="L44" s="55"/>
       <c r="M44" s="55" t="s">
         <v>103</v>
@@ -3310,13 +3310,13 @@
       <c r="M45" s="47"/>
     </row>
     <row r="46" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="145" t="s">
+      <c r="A46" s="178" t="s">
         <v>74</v>
       </c>
-      <c r="B46" s="152">
+      <c r="B46" s="184">
         <v>44459</v>
       </c>
-      <c r="C46" s="178" t="s">
+      <c r="C46" s="176" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="52" t="s">
@@ -3334,8 +3334,8 @@
       <c r="H46" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="I46" s="133"/>
-      <c r="J46" s="140"/>
+      <c r="I46" s="193"/>
+      <c r="J46" s="195"/>
       <c r="K46" s="62"/>
       <c r="L46" s="50"/>
       <c r="M46" s="50" t="s">
@@ -3343,9 +3343,9 @@
       </c>
     </row>
     <row r="47" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="146"/>
-      <c r="B47" s="152"/>
-      <c r="C47" s="178"/>
+      <c r="A47" s="179"/>
+      <c r="B47" s="184"/>
+      <c r="C47" s="176"/>
       <c r="D47" s="50" t="s">
         <v>63</v>
       </c>
@@ -3357,8 +3357,8 @@
       <c r="H47" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I47" s="135"/>
-      <c r="J47" s="142"/>
+      <c r="I47" s="199"/>
+      <c r="J47" s="200"/>
       <c r="K47" s="63"/>
       <c r="L47" s="50"/>
       <c r="M47" s="50" t="s">
@@ -3366,9 +3366,9 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="146"/>
-      <c r="B48" s="152"/>
-      <c r="C48" s="178"/>
+      <c r="A48" s="179"/>
+      <c r="B48" s="184"/>
+      <c r="C48" s="176"/>
       <c r="D48" s="50" t="s">
         <v>116</v>
       </c>
@@ -3380,8 +3380,8 @@
       <c r="H48" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="I48" s="135"/>
-      <c r="J48" s="142"/>
+      <c r="I48" s="199"/>
+      <c r="J48" s="200"/>
       <c r="K48" s="63"/>
       <c r="L48" s="50"/>
       <c r="M48" s="50" t="s">
@@ -3389,9 +3389,9 @@
       </c>
     </row>
     <row r="49" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="146"/>
-      <c r="B49" s="152"/>
-      <c r="C49" s="178"/>
+      <c r="A49" s="179"/>
+      <c r="B49" s="184"/>
+      <c r="C49" s="176"/>
       <c r="D49" s="50" t="s">
         <v>30</v>
       </c>
@@ -3407,8 +3407,8 @@
       <c r="H49" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="I49" s="134"/>
-      <c r="J49" s="141"/>
+      <c r="I49" s="194"/>
+      <c r="J49" s="196"/>
       <c r="K49" s="64"/>
       <c r="L49" s="50"/>
       <c r="M49" s="50" t="s">
@@ -3416,7 +3416,7 @@
       </c>
     </row>
     <row r="50" spans="1:14" s="69" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="146"/>
+      <c r="A50" s="179"/>
       <c r="B50" s="66">
         <v>44460</v>
       </c>
@@ -3435,11 +3435,11 @@
       <c r="M50" s="47"/>
     </row>
     <row r="51" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="146"/>
-      <c r="B51" s="153">
+      <c r="A51" s="179"/>
+      <c r="B51" s="185">
         <v>44461</v>
       </c>
-      <c r="C51" s="168" t="s">
+      <c r="C51" s="171" t="s">
         <v>13</v>
       </c>
       <c r="D51" s="54" t="s">
@@ -3457,10 +3457,10 @@
       <c r="H51" s="54" t="s">
         <v>134</v>
       </c>
-      <c r="I51" s="131" t="s">
+      <c r="I51" s="191" t="s">
         <v>101</v>
       </c>
-      <c r="J51" s="143"/>
+      <c r="J51" s="201"/>
       <c r="K51" s="98"/>
       <c r="L51" s="54"/>
       <c r="M51" s="54" t="s">
@@ -3468,9 +3468,9 @@
       </c>
     </row>
     <row r="52" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="146"/>
-      <c r="B52" s="154"/>
-      <c r="C52" s="169"/>
+      <c r="A52" s="179"/>
+      <c r="B52" s="186"/>
+      <c r="C52" s="172"/>
       <c r="D52" s="54" t="s">
         <v>59</v>
       </c>
@@ -3482,8 +3482,8 @@
       <c r="H52" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="I52" s="132"/>
-      <c r="J52" s="144"/>
+      <c r="I52" s="192"/>
+      <c r="J52" s="202"/>
       <c r="K52" s="99"/>
       <c r="L52" s="54"/>
       <c r="M52" s="54" t="s">
@@ -3491,7 +3491,7 @@
       </c>
     </row>
     <row r="53" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="146"/>
+      <c r="A53" s="179"/>
       <c r="B53" s="67">
         <v>44462</v>
       </c>
@@ -3518,11 +3518,11 @@
       </c>
     </row>
     <row r="54" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="146"/>
-      <c r="B54" s="158">
+      <c r="A54" s="179"/>
+      <c r="B54" s="187">
         <v>44463</v>
       </c>
-      <c r="C54" s="170" t="s">
+      <c r="C54" s="173" t="s">
         <v>12</v>
       </c>
       <c r="D54" s="54" t="s">
@@ -3532,16 +3532,16 @@
         <v>2</v>
       </c>
       <c r="F54" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="G54" s="54" t="s">
         <v>169</v>
-      </c>
-      <c r="G54" s="54" t="s">
-        <v>170</v>
       </c>
       <c r="H54" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="I54" s="131"/>
-      <c r="J54" s="143"/>
+      <c r="I54" s="191"/>
+      <c r="J54" s="201"/>
       <c r="K54" s="98"/>
       <c r="L54" s="55" t="s">
         <v>107</v>
@@ -3551,9 +3551,9 @@
       </c>
     </row>
     <row r="55" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="147"/>
-      <c r="B55" s="159"/>
-      <c r="C55" s="171"/>
+      <c r="A55" s="180"/>
+      <c r="B55" s="188"/>
+      <c r="C55" s="174"/>
       <c r="D55" s="54" t="s">
         <v>63</v>
       </c>
@@ -3565,8 +3565,8 @@
       <c r="H55" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="I55" s="132"/>
-      <c r="J55" s="144"/>
+      <c r="I55" s="192"/>
+      <c r="J55" s="202"/>
       <c r="K55" s="99"/>
       <c r="L55" s="54"/>
       <c r="M55" s="54" t="s">
@@ -3592,13 +3592,13 @@
       <c r="M56" s="47"/>
     </row>
     <row r="57" spans="1:14" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="148" t="s">
+      <c r="A57" s="181" t="s">
         <v>75</v>
       </c>
-      <c r="B57" s="163">
+      <c r="B57" s="189">
         <v>44466</v>
       </c>
-      <c r="C57" s="179" t="s">
+      <c r="C57" s="177" t="s">
         <v>7</v>
       </c>
       <c r="D57" s="50" t="s">
@@ -3616,8 +3616,8 @@
       <c r="H57" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="I57" s="140"/>
-      <c r="J57" s="140"/>
+      <c r="I57" s="195"/>
+      <c r="J57" s="195"/>
       <c r="K57" s="62"/>
       <c r="L57" s="50"/>
       <c r="M57" s="50" t="s">
@@ -3625,9 +3625,9 @@
       </c>
     </row>
     <row r="58" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="149"/>
-      <c r="B58" s="164"/>
-      <c r="C58" s="179"/>
+      <c r="A58" s="182"/>
+      <c r="B58" s="190"/>
+      <c r="C58" s="177"/>
       <c r="D58" s="50" t="s">
         <v>120</v>
       </c>
@@ -3639,8 +3639,8 @@
         <v>14</v>
       </c>
       <c r="H58" s="97"/>
-      <c r="I58" s="141"/>
-      <c r="J58" s="141"/>
+      <c r="I58" s="196"/>
+      <c r="J58" s="196"/>
       <c r="K58" s="64"/>
       <c r="L58" s="97"/>
       <c r="M58" s="97" t="s">
@@ -3648,7 +3648,7 @@
       </c>
     </row>
     <row r="59" spans="1:14" s="69" customFormat="1" ht="25.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="149"/>
+      <c r="A59" s="182"/>
       <c r="B59" s="66">
         <v>44467</v>
       </c>
@@ -3670,11 +3670,11 @@
       <c r="N59" s="34"/>
     </row>
     <row r="60" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="149"/>
-      <c r="B60" s="153">
+      <c r="A60" s="182"/>
+      <c r="B60" s="185">
         <v>44468</v>
       </c>
-      <c r="C60" s="167" t="s">
+      <c r="C60" s="170" t="s">
         <v>13</v>
       </c>
       <c r="D60" s="54" t="s">
@@ -3692,31 +3692,31 @@
       <c r="H60" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="I60" s="129"/>
-      <c r="J60" s="129"/>
-      <c r="K60" s="129"/>
+      <c r="I60" s="197"/>
+      <c r="J60" s="197"/>
+      <c r="K60" s="197"/>
       <c r="L60" s="57"/>
       <c r="M60" s="57" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="149"/>
-      <c r="B61" s="154"/>
-      <c r="C61" s="167"/>
+      <c r="A61" s="182"/>
+      <c r="B61" s="186"/>
+      <c r="C61" s="170"/>
       <c r="D61" s="54"/>
       <c r="E61" s="119"/>
       <c r="F61" s="57"/>
       <c r="G61" s="57"/>
       <c r="H61" s="57"/>
-      <c r="I61" s="130"/>
-      <c r="J61" s="130"/>
-      <c r="K61" s="130"/>
+      <c r="I61" s="198"/>
+      <c r="J61" s="198"/>
+      <c r="K61" s="198"/>
       <c r="L61" s="57"/>
       <c r="M61" s="57"/>
     </row>
     <row r="62" spans="1:14" ht="12.9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="149"/>
+      <c r="A62" s="182"/>
       <c r="B62" s="67">
         <v>44469</v>
       </c>
@@ -3735,7 +3735,7 @@
       <c r="M62" s="97"/>
     </row>
     <row r="63" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="149"/>
+      <c r="A63" s="182"/>
       <c r="B63" s="124">
         <v>44470</v>
       </c>
@@ -3797,32 +3797,69 @@
       <c r="M65" s="69"/>
     </row>
     <row r="66" spans="1:13" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="181" t="s">
+      <c r="A66" s="160" t="s">
         <v>92</v>
       </c>
-      <c r="B66" s="182"/>
-      <c r="C66" s="183"/>
+      <c r="B66" s="161"/>
+      <c r="C66" s="162"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M63" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="87">
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="K43:K44"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="K35:K38"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="A12:A22"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="K60:K61"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="J35:J38"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="J43:J44"/>
+    <mergeCell ref="I35:I38"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="I57:I58"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="I46:I49"/>
+    <mergeCell ref="J46:J49"/>
+    <mergeCell ref="I51:I52"/>
+    <mergeCell ref="J51:J52"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="A46:A55"/>
+    <mergeCell ref="A57:A63"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A35:A44"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C57:C58"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:J10"/>
     <mergeCell ref="A66:C66"/>
@@ -3839,60 +3876,23 @@
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="A24:A33"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="A46:A55"/>
-    <mergeCell ref="A57:A63"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A35:A44"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="I57:I58"/>
-    <mergeCell ref="J57:J58"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="I46:I49"/>
-    <mergeCell ref="J46:J49"/>
-    <mergeCell ref="I51:I52"/>
-    <mergeCell ref="J51:J52"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="K60:K61"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="J35:J38"/>
-    <mergeCell ref="J40:J41"/>
-    <mergeCell ref="J43:J44"/>
-    <mergeCell ref="I35:I38"/>
-    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A12:A22"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="K35:K38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J35" r:id="rId1" xr:uid="{6F56A95F-302D-430F-BB93-125813A81349}"/>
@@ -3989,7 +3989,7 @@
       <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="211">
+      <c r="A8" s="212">
         <v>34</v>
       </c>
       <c r="B8" s="30" t="s">
@@ -4005,8 +4005,8 @@
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="211"/>
-      <c r="B9" s="213" t="s">
+      <c r="A9" s="212"/>
+      <c r="B9" s="206" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="23" t="s">
@@ -4029,8 +4029,8 @@
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="211"/>
-      <c r="B10" s="214"/>
+      <c r="A10" s="212"/>
+      <c r="B10" s="221"/>
       <c r="C10" s="23" t="s">
         <v>22</v>
       </c>
@@ -4049,8 +4049,8 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" ht="51.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="211"/>
-      <c r="B11" s="214"/>
+      <c r="A11" s="212"/>
+      <c r="B11" s="221"/>
       <c r="C11" s="17" t="s">
         <v>35</v>
       </c>
@@ -4073,8 +4073,8 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="211"/>
-      <c r="B12" s="215"/>
+      <c r="A12" s="212"/>
+      <c r="B12" s="222"/>
       <c r="C12" s="17" t="s">
         <v>40</v>
       </c>
@@ -4093,8 +4093,8 @@
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="211"/>
-      <c r="B13" s="216" t="s">
+      <c r="A13" s="212"/>
+      <c r="B13" s="223" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="30" t="s">
@@ -4117,8 +4117,8 @@
       <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:10" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="211"/>
-      <c r="B14" s="217"/>
+      <c r="A14" s="212"/>
+      <c r="B14" s="224"/>
       <c r="C14" s="30" t="s">
         <v>22</v>
       </c>
@@ -4137,8 +4137,8 @@
       <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="211"/>
-      <c r="B15" s="218"/>
+      <c r="A15" s="212"/>
+      <c r="B15" s="225"/>
       <c r="C15" s="30" t="s">
         <v>41</v>
       </c>
@@ -4157,8 +4157,8 @@
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10" ht="52.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="211"/>
-      <c r="B16" s="213" t="s">
+      <c r="A16" s="212"/>
+      <c r="B16" s="206" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="23" t="s">
@@ -4175,8 +4175,8 @@
       <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" ht="52.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="211"/>
-      <c r="B17" s="215"/>
+      <c r="A17" s="212"/>
+      <c r="B17" s="222"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="14"/>
@@ -4191,8 +4191,8 @@
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="211"/>
-      <c r="B18" s="216" t="s">
+      <c r="A18" s="212"/>
+      <c r="B18" s="223" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="30" t="s">
@@ -4213,8 +4213,8 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="211"/>
-      <c r="B19" s="217"/>
+      <c r="A19" s="212"/>
+      <c r="B19" s="224"/>
       <c r="C19" s="30" t="s">
         <v>22</v>
       </c>
@@ -4233,8 +4233,8 @@
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="212"/>
-      <c r="B20" s="218"/>
+      <c r="A20" s="220"/>
+      <c r="B20" s="225"/>
       <c r="C20" s="30" t="s">
         <v>41</v>
       </c>
@@ -4253,10 +4253,10 @@
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="204">
+      <c r="A21" s="214">
         <v>35</v>
       </c>
-      <c r="B21" s="207" t="s">
+      <c r="B21" s="218" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="9"/>
@@ -4275,8 +4275,8 @@
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="205"/>
-      <c r="B22" s="208"/>
+      <c r="A22" s="213"/>
+      <c r="B22" s="207"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="15"/>
@@ -4289,7 +4289,7 @@
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="205"/>
+      <c r="A23" s="213"/>
       <c r="B23" s="9" t="s">
         <v>10</v>
       </c>
@@ -4303,8 +4303,8 @@
       <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="205"/>
-      <c r="B24" s="207" t="s">
+      <c r="A24" s="213"/>
+      <c r="B24" s="218" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="9"/>
@@ -4323,8 +4323,8 @@
       <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="205"/>
-      <c r="B25" s="208"/>
+      <c r="A25" s="213"/>
+      <c r="B25" s="207"/>
       <c r="C25" s="9"/>
       <c r="D25" s="15"/>
       <c r="E25" s="9"/>
@@ -4335,8 +4335,8 @@
       <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="205"/>
-      <c r="B26" s="207" t="s">
+      <c r="A26" s="213"/>
+      <c r="B26" s="218" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -4353,8 +4353,8 @@
       <c r="J26" s="11"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="205"/>
-      <c r="B27" s="208"/>
+      <c r="A27" s="213"/>
+      <c r="B27" s="207"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="15"/>
@@ -4365,8 +4365,8 @@
       <c r="J27" s="11"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="205"/>
-      <c r="B28" s="209" t="s">
+      <c r="A28" s="213"/>
+      <c r="B28" s="226" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="9"/>
@@ -4379,8 +4379,8 @@
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="206"/>
-      <c r="B29" s="210"/>
+      <c r="A29" s="217"/>
+      <c r="B29" s="227"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="21"/>
@@ -4391,10 +4391,10 @@
       <c r="J29" s="11"/>
     </row>
     <row r="30" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="224">
+      <c r="A30" s="211">
         <v>36</v>
       </c>
-      <c r="B30" s="213" t="s">
+      <c r="B30" s="206" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="23"/>
@@ -4413,8 +4413,8 @@
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="211"/>
-      <c r="B31" s="208"/>
+      <c r="A31" s="212"/>
+      <c r="B31" s="207"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
       <c r="E31" s="14"/>
@@ -4425,7 +4425,7 @@
       <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="205"/>
+      <c r="A32" s="213"/>
       <c r="B32" s="23" t="s">
         <v>10</v>
       </c>
@@ -4439,7 +4439,7 @@
       <c r="J32" s="11"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="205"/>
+      <c r="A33" s="213"/>
       <c r="B33" s="23" t="s">
         <v>13</v>
       </c>
@@ -4457,8 +4457,8 @@
       <c r="J33" s="11"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="205"/>
-      <c r="B34" s="213" t="s">
+      <c r="A34" s="213"/>
+      <c r="B34" s="206" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="23" t="s">
@@ -4475,8 +4475,8 @@
       <c r="J34" s="11"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="205"/>
-      <c r="B35" s="208"/>
+      <c r="A35" s="213"/>
+      <c r="B35" s="207"/>
       <c r="C35" s="23"/>
       <c r="D35" s="23"/>
       <c r="E35" s="14"/>
@@ -4487,8 +4487,8 @@
       <c r="J35" s="11"/>
     </row>
     <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="205"/>
-      <c r="B36" s="213" t="s">
+      <c r="A36" s="213"/>
+      <c r="B36" s="206" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="23"/>
@@ -4507,8 +4507,8 @@
       <c r="J36" s="11"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="205"/>
-      <c r="B37" s="208"/>
+      <c r="A37" s="213"/>
+      <c r="B37" s="207"/>
       <c r="C37" s="23"/>
       <c r="D37" s="23"/>
       <c r="E37" s="23"/>
@@ -4519,10 +4519,10 @@
       <c r="J37" s="11"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="204">
+      <c r="A38" s="214">
         <v>37</v>
       </c>
-      <c r="B38" s="207" t="s">
+      <c r="B38" s="218" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="9"/>
@@ -4535,8 +4535,8 @@
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="225"/>
-      <c r="B39" s="208"/>
+      <c r="A39" s="215"/>
+      <c r="B39" s="207"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="15"/>
@@ -4547,7 +4547,7 @@
       <c r="J39" s="11"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="226"/>
+      <c r="A40" s="216"/>
       <c r="B40" s="10" t="s">
         <v>10</v>
       </c>
@@ -4561,7 +4561,7 @@
       <c r="J40" s="11"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="226"/>
+      <c r="A41" s="216"/>
       <c r="B41" s="10" t="s">
         <v>13</v>
       </c>
@@ -4575,8 +4575,8 @@
       <c r="J41" s="11"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="226"/>
-      <c r="B42" s="207" t="s">
+      <c r="A42" s="216"/>
+      <c r="B42" s="218" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="9" t="s">
@@ -4593,8 +4593,8 @@
       <c r="J42" s="11"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="226"/>
-      <c r="B43" s="227"/>
+      <c r="A43" s="216"/>
+      <c r="B43" s="219"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -4605,8 +4605,8 @@
       <c r="J43" s="11"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="226"/>
-      <c r="B44" s="208"/>
+      <c r="A44" s="216"/>
+      <c r="B44" s="207"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="20"/>
@@ -4617,8 +4617,8 @@
       <c r="J44" s="11"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="226"/>
-      <c r="B45" s="207" t="s">
+      <c r="A45" s="216"/>
+      <c r="B45" s="218" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="9"/>
@@ -4631,8 +4631,8 @@
       <c r="J45" s="11"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="205"/>
-      <c r="B46" s="227"/>
+      <c r="A46" s="213"/>
+      <c r="B46" s="219"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
@@ -4643,8 +4643,8 @@
       <c r="J46" s="11"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="206"/>
-      <c r="B47" s="208"/>
+      <c r="A47" s="217"/>
+      <c r="B47" s="207"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="20"/>
@@ -4655,10 +4655,10 @@
       <c r="J47" s="11"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="219">
+      <c r="A48" s="204">
         <v>38</v>
       </c>
-      <c r="B48" s="213" t="s">
+      <c r="B48" s="206" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="23"/>
@@ -4671,8 +4671,8 @@
       <c r="J48" s="11"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="219"/>
-      <c r="B49" s="208"/>
+      <c r="A49" s="204"/>
+      <c r="B49" s="207"/>
       <c r="C49" s="23"/>
       <c r="D49" s="23"/>
       <c r="E49" s="23"/>
@@ -4683,7 +4683,7 @@
       <c r="J49" s="11"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="220"/>
+      <c r="A50" s="205"/>
       <c r="B50" s="23" t="s">
         <v>10</v>
       </c>
@@ -4697,7 +4697,7 @@
       <c r="J50" s="11"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="220"/>
+      <c r="A51" s="205"/>
       <c r="B51" s="23" t="s">
         <v>13</v>
       </c>
@@ -4711,7 +4711,7 @@
       <c r="J51" s="11"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="220"/>
+      <c r="A52" s="205"/>
       <c r="B52" s="23" t="s">
         <v>11</v>
       </c>
@@ -4729,8 +4729,8 @@
       <c r="J52" s="11"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="220"/>
-      <c r="B53" s="219" t="s">
+      <c r="A53" s="205"/>
+      <c r="B53" s="204" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="17"/>
@@ -4743,8 +4743,8 @@
       <c r="J53" s="11"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="220"/>
-      <c r="B54" s="220"/>
+      <c r="A54" s="205"/>
+      <c r="B54" s="205"/>
       <c r="C54" s="23"/>
       <c r="D54" s="23"/>
       <c r="E54" s="22"/>
@@ -4755,7 +4755,7 @@
       <c r="J54" s="11"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="221">
+      <c r="A55" s="208">
         <v>39</v>
       </c>
       <c r="B55" s="24" t="s">
@@ -4771,7 +4771,7 @@
       <c r="J55" s="11"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="222"/>
+      <c r="A56" s="209"/>
       <c r="B56" s="25" t="s">
         <v>10</v>
       </c>
@@ -4784,7 +4784,7 @@
       <c r="I56" s="28"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="222"/>
+      <c r="A57" s="209"/>
       <c r="B57" s="25" t="s">
         <v>13</v>
       </c>
@@ -4797,7 +4797,7 @@
       <c r="I57" s="28"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="222"/>
+      <c r="A58" s="209"/>
       <c r="B58" s="25" t="s">
         <v>11</v>
       </c>
@@ -4814,7 +4814,7 @@
       <c r="I58" s="28"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="223"/>
+      <c r="A59" s="210"/>
       <c r="B59" s="26" t="s">
         <v>12</v>
       </c>
@@ -4828,6 +4828,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A8:A20"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="A48:A54"/>
     <mergeCell ref="B48:B49"/>
     <mergeCell ref="B53:B54"/>
@@ -4840,16 +4850,6 @@
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
-    <mergeCell ref="A8:A20"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
list comprehension exercises for week 4
</commit_message>
<xml_diff>
--- a/01_studieplan_och_schema.xlsx
+++ b/01_studieplan_och_schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsabellaGagner\Documents\Programming-projects\EC\ec-python-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1CFC1E-E18C-4ED0-A153-F8A9E8BA7F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771F38C0-D1AF-47D2-8358-7A16DD620CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7188" yWindow="-17388" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema - Python" sheetId="1" r:id="rId1"/>
@@ -279,9 +279,6 @@
     <t>God programmeringssed, Filhantering</t>
   </si>
   <si>
-    <t>Skapa UML-diagram från förra veckans uppgifter</t>
-  </si>
-  <si>
     <t>Dataframes med Pandas</t>
   </si>
   <si>
@@ -577,6 +574,9 @@
   </si>
   <si>
     <t>git: merge conflicts</t>
+  </si>
+  <si>
+    <t>PP 16-18</t>
   </si>
 </sst>
 </file>
@@ -2013,8 +2013,8 @@
   <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I35" sqref="I35:I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1015625" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -2050,7 +2050,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F1" s="73" t="s">
         <v>3</v>
@@ -2068,7 +2068,7 @@
         <v>43</v>
       </c>
       <c r="K1" s="73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L1" s="73" t="s">
         <v>36</v>
@@ -2124,7 +2124,7 @@
         <v>55</v>
       </c>
       <c r="I3" s="184" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J3" s="184" t="s">
         <v>46</v>
@@ -2162,7 +2162,7 @@
       <c r="K4" s="79"/>
       <c r="L4" s="51"/>
       <c r="M4" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N4" s="77"/>
     </row>
@@ -2180,7 +2180,7 @@
         <v>66</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H5" s="51" t="s">
         <v>77</v>
@@ -2220,7 +2220,7 @@
         <v>57</v>
       </c>
       <c r="I6" s="180" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J6" s="180" t="s">
         <v>48</v>
@@ -2228,7 +2228,7 @@
       <c r="K6" s="56"/>
       <c r="L6" s="55"/>
       <c r="M6" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N6" s="77"/>
     </row>
@@ -2252,7 +2252,7 @@
       <c r="K7" s="56"/>
       <c r="L7" s="55"/>
       <c r="M7" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N7" s="77"/>
     </row>
@@ -2276,15 +2276,15 @@
       </c>
       <c r="H8" s="51"/>
       <c r="I8" s="61" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J8" s="61" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K8" s="61"/>
       <c r="L8" s="51"/>
       <c r="M8" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N8" s="77"/>
     </row>
@@ -2306,23 +2306,23 @@
         <v>67</v>
       </c>
       <c r="G9" s="55" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H9" s="55" t="s">
         <v>62</v>
       </c>
       <c r="I9" s="180" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J9" s="180" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K9" s="56"/>
       <c r="L9" s="131" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M9" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N9" s="77"/>
     </row>
@@ -2346,7 +2346,7 @@
       <c r="K10" s="56"/>
       <c r="L10" s="132"/>
       <c r="M10" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N10" s="77"/>
     </row>
@@ -2389,23 +2389,23 @@
         <v>28</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H12" s="50" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I12" s="137" t="s">
+        <v>160</v>
+      </c>
+      <c r="J12" s="137" t="s">
         <v>161</v>
       </c>
-      <c r="J12" s="137" t="s">
-        <v>162</v>
-      </c>
       <c r="K12" s="199" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L12" s="53"/>
       <c r="M12" s="53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N12" s="77"/>
     </row>
@@ -2429,7 +2429,7 @@
       <c r="K13" s="200"/>
       <c r="L13" s="51"/>
       <c r="M13" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N13" s="77"/>
     </row>
@@ -2438,7 +2438,7 @@
       <c r="B14" s="161"/>
       <c r="C14" s="175"/>
       <c r="D14" s="50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E14" s="116">
         <v>1</v>
@@ -2453,7 +2453,7 @@
       <c r="K14" s="200"/>
       <c r="L14" s="51"/>
       <c r="M14" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N14" s="77"/>
     </row>
@@ -2471,17 +2471,17 @@
         <v>68</v>
       </c>
       <c r="G15" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H15" s="50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I15" s="139"/>
       <c r="J15" s="139"/>
       <c r="K15" s="201"/>
       <c r="L15" s="51"/>
       <c r="M15" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N15" s="77"/>
     </row>
@@ -2499,10 +2499,10 @@
       <c r="G16" s="48"/>
       <c r="H16" s="48"/>
       <c r="I16" s="114" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J16" s="127" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K16" s="48"/>
       <c r="L16" s="48"/>
@@ -2527,21 +2527,21 @@
         <v>69</v>
       </c>
       <c r="G17" s="55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H17" s="55" t="s">
         <v>64</v>
       </c>
       <c r="I17" s="131" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J17" s="131" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K17" s="95"/>
       <c r="L17" s="131"/>
       <c r="M17" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N17" s="77"/>
     </row>
@@ -2567,7 +2567,7 @@
       <c r="K18" s="96"/>
       <c r="L18" s="132"/>
       <c r="M18" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N18" s="77"/>
     </row>
@@ -2591,15 +2591,15 @@
       </c>
       <c r="H19" s="51"/>
       <c r="I19" s="133" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J19" s="133" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K19" s="93"/>
       <c r="L19" s="133"/>
       <c r="M19" s="51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N19" s="77"/>
     </row>
@@ -2637,21 +2637,21 @@
         <v>78</v>
       </c>
       <c r="G21" s="55" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H21" s="55" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I21" s="131" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J21" s="128" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K21" s="55"/>
       <c r="L21" s="55"/>
       <c r="M21" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N21" s="77"/>
     </row>
@@ -2675,7 +2675,7 @@
       <c r="K22" s="55"/>
       <c r="L22" s="55"/>
       <c r="M22" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N22" s="77"/>
     </row>
@@ -2709,30 +2709,30 @@
         <v>7</v>
       </c>
       <c r="D24" s="53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E24" s="111">
         <v>1.5</v>
       </c>
       <c r="F24" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G24" s="51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H24" s="51" t="s">
         <v>65</v>
       </c>
       <c r="I24" s="133" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J24" s="133"/>
       <c r="K24" s="194" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L24" s="51"/>
       <c r="M24" s="51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N24" s="77"/>
     </row>
@@ -2741,13 +2741,13 @@
       <c r="B25" s="161"/>
       <c r="C25" s="175"/>
       <c r="D25" s="51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E25" s="61">
         <v>1.5</v>
       </c>
       <c r="F25" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G25" s="51"/>
       <c r="H25" s="51" t="s">
@@ -2758,7 +2758,7 @@
       <c r="K25" s="195"/>
       <c r="L25" s="51"/>
       <c r="M25" s="51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N25" s="77"/>
     </row>
@@ -2767,13 +2767,13 @@
       <c r="B26" s="161"/>
       <c r="C26" s="175"/>
       <c r="D26" s="51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E26" s="61">
         <v>1</v>
       </c>
       <c r="F26" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G26" s="51"/>
       <c r="H26" s="51" t="s">
@@ -2784,7 +2784,7 @@
       <c r="K26" s="195"/>
       <c r="L26" s="51"/>
       <c r="M26" s="51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N26" s="77"/>
     </row>
@@ -2802,17 +2802,17 @@
         <v>29</v>
       </c>
       <c r="G27" s="51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H27" s="51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I27" s="135"/>
       <c r="J27" s="135"/>
       <c r="K27" s="196"/>
       <c r="L27" s="51"/>
       <c r="M27" s="51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N27" s="77"/>
     </row>
@@ -2830,7 +2830,7 @@
       <c r="G28" s="48"/>
       <c r="H28" s="48"/>
       <c r="I28" s="48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J28" s="48"/>
       <c r="K28" s="48"/>
@@ -2852,26 +2852,26 @@
         <v>2</v>
       </c>
       <c r="F29" s="55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G29" s="55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H29" s="55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I29" s="131" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J29" s="131" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K29" s="202" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L29" s="55"/>
       <c r="M29" s="55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N29" s="77"/>
     </row>
@@ -2886,7 +2886,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G30" s="55"/>
       <c r="H30" s="55" t="s">
@@ -2897,7 +2897,7 @@
       <c r="K30" s="203"/>
       <c r="L30" s="55"/>
       <c r="M30" s="55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N30" s="87"/>
     </row>
@@ -2925,7 +2925,7 @@
       <c r="K31" s="51"/>
       <c r="L31" s="51"/>
       <c r="M31" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N31" s="77"/>
     </row>
@@ -2944,16 +2944,16 @@
         <v>2</v>
       </c>
       <c r="F32" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="G32" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="G32" s="65" t="s">
-        <v>86</v>
-      </c>
       <c r="H32" s="55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I32" s="131" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J32" s="131"/>
       <c r="K32" s="95"/>
@@ -2972,7 +2972,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G33" s="55"/>
       <c r="H33" s="55" t="s">
@@ -3024,23 +3024,23 @@
         <v>29</v>
       </c>
       <c r="G35" s="51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H35" s="50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I35" s="137" t="s">
-        <v>79</v>
+        <v>178</v>
       </c>
       <c r="J35" s="136" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K35" s="137" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L35" s="51"/>
       <c r="M35" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="12.9" x14ac:dyDescent="0.55000000000000004">
@@ -3063,7 +3063,7 @@
       <c r="K36" s="138"/>
       <c r="L36" s="51"/>
       <c r="M36" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N36" s="77"/>
     </row>
@@ -3072,7 +3072,7 @@
       <c r="B37" s="161"/>
       <c r="C37" s="175"/>
       <c r="D37" s="50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E37" s="116">
         <v>1</v>
@@ -3087,7 +3087,7 @@
       <c r="K37" s="138"/>
       <c r="L37" s="51"/>
       <c r="M37" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N37" s="77"/>
     </row>
@@ -3102,20 +3102,20 @@
         <v>2</v>
       </c>
       <c r="F38" s="51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G38" s="51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H38" s="50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I38" s="139"/>
       <c r="J38" s="134"/>
       <c r="K38" s="139"/>
       <c r="L38" s="51"/>
       <c r="M38" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N38" s="77"/>
     </row>
@@ -3157,17 +3157,17 @@
         <v>76</v>
       </c>
       <c r="G40" s="55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H40" s="55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I40" s="131"/>
       <c r="J40" s="131"/>
       <c r="K40" s="95"/>
       <c r="L40" s="55"/>
       <c r="M40" s="55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3190,7 +3190,7 @@
       <c r="K41" s="96"/>
       <c r="L41" s="55"/>
       <c r="M41" s="55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N41" s="77"/>
     </row>
@@ -3218,7 +3218,7 @@
       <c r="K42" s="51"/>
       <c r="L42" s="51"/>
       <c r="M42" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N42" s="77"/>
     </row>
@@ -3240,19 +3240,19 @@
         <v>76</v>
       </c>
       <c r="G43" s="55" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H43" s="55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I43" s="131"/>
       <c r="J43" s="131"/>
       <c r="K43" s="197" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L43" s="55"/>
       <c r="M43" s="55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N43" s="77"/>
     </row>
@@ -3276,7 +3276,7 @@
       <c r="K44" s="198"/>
       <c r="L44" s="55"/>
       <c r="M44" s="55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N44" s="77"/>
     </row>
@@ -3315,20 +3315,20 @@
         <v>2</v>
       </c>
       <c r="F46" s="50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G46" s="50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H46" s="50" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I46" s="133"/>
       <c r="J46" s="140"/>
       <c r="K46" s="62"/>
       <c r="L46" s="50"/>
       <c r="M46" s="50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3351,7 +3351,7 @@
       <c r="K47" s="63"/>
       <c r="L47" s="50"/>
       <c r="M47" s="50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3359,7 +3359,7 @@
       <c r="B48" s="152"/>
       <c r="C48" s="178"/>
       <c r="D48" s="50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E48" s="116">
         <v>1</v>
@@ -3374,7 +3374,7 @@
       <c r="K48" s="63"/>
       <c r="L48" s="50"/>
       <c r="M48" s="50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3388,20 +3388,20 @@
         <v>2</v>
       </c>
       <c r="F49" s="50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G49" s="50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H49" s="50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I49" s="134"/>
       <c r="J49" s="141"/>
       <c r="K49" s="64"/>
       <c r="L49" s="50"/>
       <c r="M49" s="50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:14" s="69" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3438,22 +3438,22 @@
         <v>2</v>
       </c>
       <c r="F51" s="54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G51" s="54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H51" s="54" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I51" s="131" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J51" s="143"/>
       <c r="K51" s="98"/>
       <c r="L51" s="54"/>
       <c r="M51" s="54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3476,7 +3476,7 @@
       <c r="K52" s="99"/>
       <c r="L52" s="54"/>
       <c r="M52" s="54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3488,7 +3488,7 @@
         <v>11</v>
       </c>
       <c r="D53" s="50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E53" s="116">
         <v>4</v>
@@ -3503,7 +3503,7 @@
       <c r="K53" s="50"/>
       <c r="L53" s="50"/>
       <c r="M53" s="50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3521,22 +3521,22 @@
         <v>2</v>
       </c>
       <c r="F54" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="G54" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="G54" s="54" t="s">
-        <v>168</v>
-      </c>
       <c r="H54" s="54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I54" s="131"/>
       <c r="J54" s="143"/>
       <c r="K54" s="98"/>
       <c r="L54" s="55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M54" s="54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3559,7 +3559,7 @@
       <c r="K55" s="99"/>
       <c r="L55" s="54"/>
       <c r="M55" s="54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:14" s="69" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3597,20 +3597,20 @@
         <v>2</v>
       </c>
       <c r="F57" s="50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G57" s="51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H57" s="50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I57" s="140"/>
       <c r="J57" s="140"/>
       <c r="K57" s="62"/>
       <c r="L57" s="50"/>
       <c r="M57" s="50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3618,7 +3618,7 @@
       <c r="B58" s="164"/>
       <c r="C58" s="179"/>
       <c r="D58" s="50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E58" s="116">
         <v>3</v>
@@ -3633,7 +3633,7 @@
       <c r="K58" s="64"/>
       <c r="L58" s="97"/>
       <c r="M58" s="97" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:14" s="69" customFormat="1" ht="25.8" x14ac:dyDescent="0.55000000000000004">
@@ -3652,7 +3652,7 @@
       <c r="I59" s="70"/>
       <c r="J59" s="70"/>
       <c r="K59" s="109" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L59" s="70"/>
       <c r="M59" s="70"/>
@@ -3667,26 +3667,26 @@
         <v>13</v>
       </c>
       <c r="D60" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E60" s="119">
         <v>3</v>
       </c>
       <c r="F60" s="57" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G60" s="57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H60" s="57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I60" s="129"/>
       <c r="J60" s="129"/>
       <c r="K60" s="129"/>
       <c r="L60" s="57"/>
       <c r="M60" s="57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3732,24 +3732,24 @@
         <v>12</v>
       </c>
       <c r="D63" s="55" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E63" s="119">
         <v>4</v>
       </c>
       <c r="F63" s="57"/>
       <c r="G63" s="57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H63" s="57"/>
       <c r="I63" s="123"/>
       <c r="J63" s="123"/>
       <c r="K63" s="126" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L63" s="108"/>
       <c r="M63" s="57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="12.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3787,7 +3787,7 @@
     </row>
     <row r="66" spans="1:13" ht="13.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="181" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B66" s="182"/>
       <c r="C66" s="183"/>
@@ -4876,13 +4876,13 @@
     </row>
     <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="113" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>140</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>141</v>
       </c>
       <c r="D2" s="37"/>
     </row>
@@ -4964,24 +4964,24 @@
     </row>
     <row r="2" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="41" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="41" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>139</v>
-      </c>
       <c r="C3" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">

</xml_diff>